<commit_message>
CIERRE 1 JUL 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/BALANCE    ZAVALETA   JUNIO    2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/BALANCE    ZAVALETA   JUNIO    2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="16" activeTab="17"/>
+    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="17" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="OCTUBRE      2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -710,7 +710,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="939">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -3525,6 +3525,21 @@
   </si>
   <si>
     <t>QUESOS-POLLO-SALCHICHA-FILETE-CALAFIA</t>
+  </si>
+  <si>
+    <t>POLLO-LONGANIZA-JAMON-SALCHICHA-CHISTORRA</t>
+  </si>
+  <si>
+    <t>QUESOS-POLLO-LONGANIZA-CHORIZO</t>
+  </si>
+  <si>
+    <t>PICAÑA-QUSOS-POLLO-CREMA-MANTEQUILLA</t>
+  </si>
+  <si>
+    <t>POLLO-QUESOS-PAN ARABE</t>
+  </si>
+  <si>
+    <t>NOMINA # 25</t>
   </si>
 </sst>
 </file>
@@ -6898,39 +6913,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7003,10 +6985,76 @@
     <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -7050,39 +7098,6 @@
     </xf>
     <xf numFmtId="44" fontId="41" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7276,20 +7291,20 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="11" fillId="18" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -11684,23 +11699,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="667"/>
-      <c r="C1" s="669" t="s">
+      <c r="B1" s="691"/>
+      <c r="C1" s="693" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="670"/>
-      <c r="E1" s="670"/>
-      <c r="F1" s="670"/>
-      <c r="G1" s="670"/>
-      <c r="H1" s="670"/>
-      <c r="I1" s="670"/>
-      <c r="J1" s="670"/>
-      <c r="K1" s="670"/>
-      <c r="L1" s="670"/>
-      <c r="M1" s="670"/>
+      <c r="D1" s="694"/>
+      <c r="E1" s="694"/>
+      <c r="F1" s="694"/>
+      <c r="G1" s="694"/>
+      <c r="H1" s="694"/>
+      <c r="I1" s="694"/>
+      <c r="J1" s="694"/>
+      <c r="K1" s="694"/>
+      <c r="L1" s="694"/>
+      <c r="M1" s="694"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="668"/>
+      <c r="B2" s="692"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -11710,17 +11725,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="671" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="672"/>
+      <c r="B3" s="695" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="696"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="673" t="s">
+      <c r="H3" s="697" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="673"/>
+      <c r="I3" s="697"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -11734,14 +11749,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="674" t="s">
+      <c r="E4" s="698" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="675"/>
-      <c r="H4" s="676" t="s">
+      <c r="F4" s="699"/>
+      <c r="H4" s="700" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="677"/>
+      <c r="I4" s="701"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -11751,10 +11766,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="683" t="s">
+      <c r="P4" s="672" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="684"/>
+      <c r="Q4" s="673"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -13195,11 +13210,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="685">
+      <c r="M39" s="674">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="687">
+      <c r="N39" s="676">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -13225,8 +13240,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="686"/>
-      <c r="N40" s="688"/>
+      <c r="M40" s="675"/>
+      <c r="N40" s="677"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -13441,29 +13456,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="689" t="s">
+      <c r="H52" s="678" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="690"/>
+      <c r="I52" s="679"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="691">
+      <c r="K52" s="680">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="692"/>
-      <c r="M52" s="693">
+      <c r="L52" s="681"/>
+      <c r="M52" s="682">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="694"/>
+      <c r="N52" s="683"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="695" t="s">
+      <c r="D53" s="684" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="695"/>
+      <c r="E53" s="684"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -13474,22 +13489,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="695" t="s">
+      <c r="D54" s="684" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="695"/>
+      <c r="E54" s="684"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="696" t="s">
+      <c r="I54" s="685" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="697"/>
-      <c r="K54" s="698">
+      <c r="J54" s="686"/>
+      <c r="K54" s="687">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="699"/>
+      <c r="L54" s="688"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -13522,11 +13537,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="700">
+      <c r="K56" s="689">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="701"/>
+      <c r="L56" s="690"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -13543,22 +13558,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="678" t="s">
+      <c r="D58" s="667" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="679"/>
+      <c r="E58" s="668"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="680" t="s">
+      <c r="I58" s="669" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="681"/>
-      <c r="K58" s="682">
+      <c r="J58" s="670"/>
+      <c r="K58" s="671">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="682"/>
+      <c r="L58" s="671"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -13702,6 +13717,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -13716,12 +13737,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -16580,7 +16595,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="667"/>
+      <c r="B1" s="691"/>
       <c r="C1" s="733" t="s">
         <v>451</v>
       </c>
@@ -16596,7 +16611,7 @@
       <c r="M1" s="734"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="668"/>
+      <c r="B2" s="692"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -16606,21 +16621,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="671" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="672"/>
+      <c r="B3" s="695" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="696"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="673" t="s">
+      <c r="H3" s="697" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="673"/>
+      <c r="I3" s="697"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="710" t="s">
+      <c r="P3" s="721" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="731" t="s">
@@ -16638,14 +16653,14 @@
       <c r="D4" s="18">
         <v>44619</v>
       </c>
-      <c r="E4" s="674" t="s">
+      <c r="E4" s="698" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="675"/>
-      <c r="H4" s="676" t="s">
+      <c r="F4" s="699"/>
+      <c r="H4" s="700" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="677"/>
+      <c r="I4" s="701"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -16655,15 +16670,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="711"/>
+      <c r="P4" s="722"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="732"/>
-      <c r="W4" s="720" t="s">
+      <c r="W4" s="704" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="720"/>
+      <c r="X4" s="704"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -16714,8 +16729,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="720"/>
-      <c r="X5" s="720"/>
+      <c r="W5" s="704"/>
+      <c r="X5" s="704"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -17478,7 +17493,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="724">
+      <c r="W19" s="708">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -17530,7 +17545,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="725"/>
+      <c r="W20" s="709"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -17579,8 +17594,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="726"/>
-      <c r="X21" s="726"/>
+      <c r="W21" s="710"/>
+      <c r="X21" s="710"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -17680,8 +17695,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="727"/>
-      <c r="X23" s="727"/>
+      <c r="W23" s="711"/>
+      <c r="X23" s="711"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -17736,8 +17751,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="727"/>
-      <c r="X24" s="727"/>
+      <c r="W24" s="711"/>
+      <c r="X24" s="711"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -17785,8 +17800,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="728"/>
-      <c r="X25" s="728"/>
+      <c r="W25" s="712"/>
+      <c r="X25" s="712"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -17835,8 +17850,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="728"/>
-      <c r="X26" s="728"/>
+      <c r="W26" s="712"/>
+      <c r="X26" s="712"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -17884,9 +17899,9 @@
       <c r="R27" s="388">
         <v>170</v>
       </c>
-      <c r="W27" s="721"/>
-      <c r="X27" s="722"/>
-      <c r="Y27" s="723"/>
+      <c r="W27" s="705"/>
+      <c r="X27" s="706"/>
+      <c r="Y27" s="707"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -17934,9 +17949,9 @@
       <c r="R28" s="388">
         <v>37374.36</v>
       </c>
-      <c r="W28" s="722"/>
-      <c r="X28" s="722"/>
-      <c r="Y28" s="723"/>
+      <c r="W28" s="706"/>
+      <c r="X28" s="706"/>
+      <c r="Y28" s="707"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -18268,11 +18283,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="712">
+      <c r="M36" s="723">
         <f>SUM(M5:M35)</f>
         <v>2220612.02</v>
       </c>
-      <c r="N36" s="714">
+      <c r="N36" s="725">
         <f>SUM(N5:N35)</f>
         <v>833865</v>
       </c>
@@ -18305,8 +18320,8 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="713"/>
-      <c r="N37" s="715"/>
+      <c r="M37" s="724"/>
+      <c r="N37" s="726"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
@@ -18993,26 +19008,26 @@
       <c r="A68" s="98"/>
       <c r="B68" s="99"/>
       <c r="C68" s="1"/>
-      <c r="H68" s="689" t="s">
+      <c r="H68" s="678" t="s">
         <v>11</v>
       </c>
-      <c r="I68" s="690"/>
+      <c r="I68" s="679"/>
       <c r="J68" s="100"/>
-      <c r="K68" s="691">
+      <c r="K68" s="680">
         <f>I66+L66</f>
         <v>314868.39999999997</v>
       </c>
-      <c r="L68" s="718"/>
+      <c r="L68" s="713"/>
       <c r="M68" s="272"/>
       <c r="N68" s="272"/>
       <c r="P68" s="34"/>
       <c r="Q68" s="13"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D69" s="695" t="s">
+      <c r="D69" s="684" t="s">
         <v>12</v>
       </c>
-      <c r="E69" s="695"/>
+      <c r="E69" s="684"/>
       <c r="F69" s="312">
         <f>F66-K68-C66</f>
         <v>1594593.8500000003</v>
@@ -19021,22 +19036,22 @@
       <c r="J69" s="103"/>
     </row>
     <row r="70" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D70" s="719" t="s">
+      <c r="D70" s="714" t="s">
         <v>95</v>
       </c>
-      <c r="E70" s="719"/>
+      <c r="E70" s="714"/>
       <c r="F70" s="111">
         <v>-1360260.32</v>
       </c>
-      <c r="I70" s="696" t="s">
+      <c r="I70" s="685" t="s">
         <v>13</v>
       </c>
-      <c r="J70" s="697"/>
-      <c r="K70" s="698">
+      <c r="J70" s="686"/>
+      <c r="K70" s="687">
         <f>F72+F73+F74</f>
         <v>1938640.11</v>
       </c>
-      <c r="L70" s="698"/>
+      <c r="L70" s="687"/>
       <c r="M70" s="404"/>
       <c r="N70" s="404"/>
       <c r="O70" s="404"/>
@@ -19077,11 +19092,11 @@
         <v>15</v>
       </c>
       <c r="J72" s="109"/>
-      <c r="K72" s="700">
+      <c r="K72" s="689">
         <f>-C4</f>
         <v>-1266568.45</v>
       </c>
-      <c r="L72" s="701"/>
+      <c r="L72" s="690"/>
     </row>
     <row r="73" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D73" s="110" t="s">
@@ -19098,22 +19113,22 @@
       <c r="C74" s="112">
         <v>44647</v>
       </c>
-      <c r="D74" s="678" t="s">
+      <c r="D74" s="667" t="s">
         <v>18</v>
       </c>
-      <c r="E74" s="679"/>
+      <c r="E74" s="668"/>
       <c r="F74" s="113">
         <v>1792817.68</v>
       </c>
-      <c r="I74" s="680" t="s">
+      <c r="I74" s="669" t="s">
         <v>198</v>
       </c>
-      <c r="J74" s="681"/>
-      <c r="K74" s="682">
+      <c r="J74" s="670"/>
+      <c r="K74" s="671">
         <f>K70+K72</f>
         <v>672071.66000000015</v>
       </c>
-      <c r="L74" s="682"/>
+      <c r="L74" s="671"/>
     </row>
     <row r="75" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C75" s="114"/>
@@ -19260,6 +19275,21 @@
     <sortCondition ref="B34:B42"/>
   </sortState>
   <mergeCells count="30">
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="M39:N39"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -19275,21 +19305,6 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
   </mergeCells>
   <pageMargins left="0.27559055118110237" right="0.15748031496062992" top="0.39370078740157483" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -21875,7 +21890,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="667"/>
+      <c r="B1" s="691"/>
       <c r="C1" s="733" t="s">
         <v>620</v>
       </c>
@@ -21891,7 +21906,7 @@
       <c r="M1" s="734"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="668"/>
+      <c r="B2" s="692"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -21901,21 +21916,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="671" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="672"/>
+      <c r="B3" s="695" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="696"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="673" t="s">
+      <c r="H3" s="697" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="673"/>
+      <c r="I3" s="697"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="710" t="s">
+      <c r="P3" s="721" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="731" t="s">
@@ -21933,14 +21948,14 @@
       <c r="D4" s="18">
         <v>44647</v>
       </c>
-      <c r="E4" s="674" t="s">
+      <c r="E4" s="698" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="675"/>
-      <c r="H4" s="676" t="s">
+      <c r="F4" s="699"/>
+      <c r="H4" s="700" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="677"/>
+      <c r="I4" s="701"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -21950,15 +21965,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="711"/>
+      <c r="P4" s="722"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="732"/>
-      <c r="W4" s="720" t="s">
+      <c r="W4" s="704" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="720"/>
+      <c r="X4" s="704"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -22009,8 +22024,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="720"/>
-      <c r="X5" s="720"/>
+      <c r="W5" s="704"/>
+      <c r="X5" s="704"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -22769,7 +22784,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="724">
+      <c r="W19" s="708">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -22821,7 +22836,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="725"/>
+      <c r="W20" s="709"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -22870,8 +22885,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="726"/>
-      <c r="X21" s="726"/>
+      <c r="W21" s="710"/>
+      <c r="X21" s="710"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -22968,8 +22983,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="727"/>
-      <c r="X23" s="727"/>
+      <c r="W23" s="711"/>
+      <c r="X23" s="711"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -23024,8 +23039,8 @@
         <v>642</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="727"/>
-      <c r="X24" s="727"/>
+      <c r="W24" s="711"/>
+      <c r="X24" s="711"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -23071,8 +23086,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="728"/>
-      <c r="X25" s="728"/>
+      <c r="W25" s="712"/>
+      <c r="X25" s="712"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -23123,8 +23138,8 @@
       <c r="R26" s="388">
         <v>73524.61</v>
       </c>
-      <c r="W26" s="728"/>
-      <c r="X26" s="728"/>
+      <c r="W26" s="712"/>
+      <c r="X26" s="712"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -23175,9 +23190,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="721"/>
-      <c r="X27" s="722"/>
-      <c r="Y27" s="723"/>
+      <c r="W27" s="705"/>
+      <c r="X27" s="706"/>
+      <c r="Y27" s="707"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -23227,9 +23242,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="722"/>
-      <c r="X28" s="722"/>
-      <c r="Y28" s="723"/>
+      <c r="W28" s="706"/>
+      <c r="X28" s="706"/>
+      <c r="Y28" s="707"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -23833,11 +23848,11 @@
       <c r="L41" s="627">
         <v>15798.5</v>
       </c>
-      <c r="M41" s="712">
+      <c r="M41" s="723">
         <f>SUM(M5:M40)</f>
         <v>2479367.6100000003</v>
       </c>
-      <c r="N41" s="712">
+      <c r="N41" s="723">
         <f>SUM(N5:N40)</f>
         <v>1195667</v>
       </c>
@@ -23875,8 +23890,8 @@
       <c r="L42" s="630">
         <v>15298.5</v>
       </c>
-      <c r="M42" s="713"/>
-      <c r="N42" s="713"/>
+      <c r="M42" s="724"/>
+      <c r="N42" s="724"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="772"/>
     </row>
@@ -24563,26 +24578,26 @@
       <c r="A70" s="98"/>
       <c r="B70" s="99"/>
       <c r="C70" s="1"/>
-      <c r="H70" s="689" t="s">
+      <c r="H70" s="678" t="s">
         <v>11</v>
       </c>
-      <c r="I70" s="690"/>
+      <c r="I70" s="679"/>
       <c r="J70" s="100"/>
-      <c r="K70" s="691">
+      <c r="K70" s="680">
         <f>I68+L68</f>
         <v>428155.54000000004</v>
       </c>
-      <c r="L70" s="718"/>
+      <c r="L70" s="713"/>
       <c r="M70" s="272"/>
       <c r="N70" s="272"/>
       <c r="P70" s="34"/>
       <c r="Q70" s="13"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D71" s="695" t="s">
+      <c r="D71" s="684" t="s">
         <v>12</v>
       </c>
-      <c r="E71" s="695"/>
+      <c r="E71" s="684"/>
       <c r="F71" s="312">
         <f>F68-K70-C68</f>
         <v>1631087.67</v>
@@ -24592,22 +24607,22 @@
       <c r="P71" s="34"/>
     </row>
     <row r="72" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D72" s="719" t="s">
+      <c r="D72" s="714" t="s">
         <v>95</v>
       </c>
-      <c r="E72" s="719"/>
+      <c r="E72" s="714"/>
       <c r="F72" s="111">
         <v>-1884975.46</v>
       </c>
-      <c r="I72" s="696" t="s">
+      <c r="I72" s="685" t="s">
         <v>13</v>
       </c>
-      <c r="J72" s="697"/>
-      <c r="K72" s="698">
+      <c r="J72" s="686"/>
+      <c r="K72" s="687">
         <f>F74+F75+F76</f>
         <v>1777829.89</v>
       </c>
-      <c r="L72" s="698"/>
+      <c r="L72" s="687"/>
       <c r="M72" s="404"/>
       <c r="N72" s="404"/>
       <c r="O72" s="404"/>
@@ -24648,11 +24663,11 @@
         <v>15</v>
       </c>
       <c r="J74" s="109"/>
-      <c r="K74" s="700">
+      <c r="K74" s="689">
         <f>-C4</f>
         <v>-1792817.68</v>
       </c>
-      <c r="L74" s="701"/>
+      <c r="L74" s="690"/>
       <c r="P74" s="34"/>
     </row>
     <row r="75" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -24671,22 +24686,22 @@
       <c r="C76" s="112">
         <v>44682</v>
       </c>
-      <c r="D76" s="678" t="s">
+      <c r="D76" s="667" t="s">
         <v>18</v>
       </c>
-      <c r="E76" s="679"/>
+      <c r="E76" s="668"/>
       <c r="F76" s="113">
         <v>2112071.92</v>
       </c>
-      <c r="I76" s="680" t="s">
+      <c r="I76" s="669" t="s">
         <v>854</v>
       </c>
-      <c r="J76" s="681"/>
-      <c r="K76" s="682">
+      <c r="J76" s="670"/>
+      <c r="K76" s="671">
         <f>K72+K74</f>
         <v>-14987.790000000037</v>
       </c>
-      <c r="L76" s="682"/>
+      <c r="L76" s="671"/>
       <c r="P76" s="34"/>
     </row>
     <row r="77" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
@@ -24846,6 +24861,21 @@
     <sortCondition ref="J47:J67"/>
   </sortState>
   <mergeCells count="30">
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="M45:N45"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -24861,21 +24891,6 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="K72:L72"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -28172,7 +28187,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="667"/>
+      <c r="B1" s="691"/>
       <c r="C1" s="733" t="s">
         <v>754</v>
       </c>
@@ -28188,7 +28203,7 @@
       <c r="M1" s="734"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="668"/>
+      <c r="B2" s="692"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -28198,21 +28213,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="671" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="672"/>
+      <c r="B3" s="695" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="696"/>
       <c r="D3" s="10"/>
       <c r="E3" s="556"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="673" t="s">
+      <c r="H3" s="697" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="673"/>
+      <c r="I3" s="697"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="710" t="s">
+      <c r="P3" s="721" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="731" t="s">
@@ -28234,14 +28249,14 @@
       <c r="D4" s="18">
         <v>44682</v>
       </c>
-      <c r="E4" s="674" t="s">
+      <c r="E4" s="698" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="675"/>
-      <c r="H4" s="676" t="s">
+      <c r="F4" s="699"/>
+      <c r="H4" s="700" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="677"/>
+      <c r="I4" s="701"/>
       <c r="J4" s="559"/>
       <c r="K4" s="565"/>
       <c r="L4" s="566"/>
@@ -28251,15 +28266,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="711"/>
+      <c r="P4" s="722"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="732"/>
       <c r="U4" s="34"/>
       <c r="V4" s="128"/>
-      <c r="W4" s="793"/>
-      <c r="X4" s="793"/>
+      <c r="W4" s="796"/>
+      <c r="X4" s="796"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -28313,8 +28328,8 @@
       <c r="S5" s="324"/>
       <c r="U5" s="34"/>
       <c r="V5" s="128"/>
-      <c r="W5" s="793"/>
-      <c r="X5" s="793"/>
+      <c r="W5" s="796"/>
+      <c r="X5" s="796"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -29080,7 +29095,7 @@
       <c r="S19" s="147"/>
       <c r="U19" s="34"/>
       <c r="V19" s="128"/>
-      <c r="W19" s="794"/>
+      <c r="W19" s="797"/>
       <c r="X19" s="544"/>
       <c r="Y19" s="233"/>
     </row>
@@ -29134,7 +29149,7 @@
       <c r="S20" s="147"/>
       <c r="U20" s="34"/>
       <c r="V20" s="128"/>
-      <c r="W20" s="794"/>
+      <c r="W20" s="797"/>
       <c r="X20" s="34"/>
       <c r="Y20" s="233"/>
     </row>
@@ -29189,8 +29204,8 @@
       <c r="S21" s="147"/>
       <c r="U21" s="34"/>
       <c r="V21" s="128"/>
-      <c r="W21" s="726"/>
-      <c r="X21" s="726"/>
+      <c r="W21" s="710"/>
+      <c r="X21" s="710"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -29301,8 +29316,8 @@
       <c r="S23" s="147"/>
       <c r="U23" s="34"/>
       <c r="V23" s="128"/>
-      <c r="W23" s="727"/>
-      <c r="X23" s="727"/>
+      <c r="W23" s="711"/>
+      <c r="X23" s="711"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -29363,8 +29378,8 @@
       <c r="S24" s="147"/>
       <c r="U24" s="34"/>
       <c r="V24" s="128"/>
-      <c r="W24" s="727"/>
-      <c r="X24" s="727"/>
+      <c r="W24" s="711"/>
+      <c r="X24" s="711"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -29417,8 +29432,8 @@
       </c>
       <c r="U25" s="34"/>
       <c r="V25" s="128"/>
-      <c r="W25" s="728"/>
-      <c r="X25" s="728"/>
+      <c r="W25" s="712"/>
+      <c r="X25" s="712"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -29473,8 +29488,8 @@
       <c r="T26" s="128"/>
       <c r="U26" s="34"/>
       <c r="V26" s="128"/>
-      <c r="W26" s="728"/>
-      <c r="X26" s="728"/>
+      <c r="W26" s="712"/>
+      <c r="X26" s="712"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -29529,9 +29544,9 @@
       <c r="T27" s="128"/>
       <c r="U27" s="34"/>
       <c r="V27" s="128"/>
-      <c r="W27" s="721"/>
-      <c r="X27" s="722"/>
-      <c r="Y27" s="723"/>
+      <c r="W27" s="705"/>
+      <c r="X27" s="706"/>
+      <c r="Y27" s="707"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -29585,9 +29600,9 @@
       <c r="T28" s="128"/>
       <c r="U28" s="34"/>
       <c r="V28" s="128"/>
-      <c r="W28" s="722"/>
-      <c r="X28" s="722"/>
-      <c r="Y28" s="723"/>
+      <c r="W28" s="706"/>
+      <c r="X28" s="706"/>
+      <c r="Y28" s="707"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -30178,11 +30193,11 @@
       <c r="J41" s="56"/>
       <c r="K41" s="38"/>
       <c r="L41" s="39"/>
-      <c r="M41" s="712">
+      <c r="M41" s="723">
         <f>SUM(M5:M40)</f>
         <v>1509924.1</v>
       </c>
-      <c r="N41" s="712">
+      <c r="N41" s="723">
         <f>SUM(N5:N40)</f>
         <v>1012291</v>
       </c>
@@ -30214,8 +30229,8 @@
       <c r="L42" s="641">
         <v>3095.88</v>
       </c>
-      <c r="M42" s="713"/>
-      <c r="N42" s="713"/>
+      <c r="M42" s="724"/>
+      <c r="N42" s="724"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="772"/>
     </row>
@@ -30706,26 +30721,26 @@
       <c r="A63" s="98"/>
       <c r="B63" s="99"/>
       <c r="C63" s="1"/>
-      <c r="H63" s="689" t="s">
+      <c r="H63" s="678" t="s">
         <v>11</v>
       </c>
-      <c r="I63" s="690"/>
+      <c r="I63" s="679"/>
       <c r="J63" s="562"/>
-      <c r="K63" s="796">
+      <c r="K63" s="793">
         <f>I61+L61</f>
         <v>340912.75</v>
       </c>
-      <c r="L63" s="797"/>
+      <c r="L63" s="794"/>
       <c r="M63" s="272"/>
       <c r="N63" s="272"/>
       <c r="P63" s="34"/>
       <c r="Q63" s="13"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D64" s="695" t="s">
+      <c r="D64" s="684" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="695"/>
+      <c r="E64" s="684"/>
       <c r="F64" s="312">
         <f>F61-K63-C61</f>
         <v>1458827.53</v>
@@ -30734,22 +30749,22 @@
       <c r="J64" s="563"/>
     </row>
     <row r="65" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D65" s="719" t="s">
+      <c r="D65" s="714" t="s">
         <v>95</v>
       </c>
-      <c r="E65" s="719"/>
+      <c r="E65" s="714"/>
       <c r="F65" s="111">
         <v>-1572197.3</v>
       </c>
-      <c r="I65" s="696" t="s">
+      <c r="I65" s="685" t="s">
         <v>13</v>
       </c>
-      <c r="J65" s="697"/>
-      <c r="K65" s="698">
+      <c r="J65" s="686"/>
+      <c r="K65" s="687">
         <f>F67+F68+F69</f>
         <v>2392765.5300000003</v>
       </c>
-      <c r="L65" s="698"/>
+      <c r="L65" s="687"/>
       <c r="M65" s="404"/>
       <c r="N65" s="404"/>
       <c r="O65" s="582"/>
@@ -30794,7 +30809,7 @@
         <f>-C4</f>
         <v>-2112071.92</v>
       </c>
-      <c r="L67" s="698"/>
+      <c r="L67" s="687"/>
     </row>
     <row r="68" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="110" t="s">
@@ -30811,22 +30826,22 @@
       <c r="C69" s="112">
         <v>44710</v>
       </c>
-      <c r="D69" s="678" t="s">
+      <c r="D69" s="667" t="s">
         <v>18</v>
       </c>
-      <c r="E69" s="679"/>
+      <c r="E69" s="668"/>
       <c r="F69" s="113">
         <v>2546982.16</v>
       </c>
-      <c r="I69" s="680" t="s">
+      <c r="I69" s="669" t="s">
         <v>198</v>
       </c>
-      <c r="J69" s="681"/>
-      <c r="K69" s="682">
+      <c r="J69" s="670"/>
+      <c r="K69" s="671">
         <f>K65+K67</f>
         <v>280693.61000000034</v>
       </c>
-      <c r="L69" s="682"/>
+      <c r="L69" s="671"/>
     </row>
     <row r="70" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C70" s="114"/>
@@ -30973,21 +30988,6 @@
     <sortCondition ref="J42:J56"/>
   </sortState>
   <mergeCells count="30">
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="K69:L69"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="K63:L63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="K65:L65"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="K67:L67"/>
-    <mergeCell ref="M45:N45"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -31003,6 +31003,21 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="K65:L65"/>
   </mergeCells>
   <pageMargins left="0.28000000000000003" right="0.19" top="0.33" bottom="0.33" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -33360,8 +33375,8 @@
   </sheetPr>
   <dimension ref="A1:Z91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19:O20"/>
+    <sheetView tabSelected="1" topLeftCell="G15" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -33391,7 +33406,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="667"/>
+      <c r="B1" s="691"/>
       <c r="C1" s="733" t="s">
         <v>886</v>
       </c>
@@ -33407,7 +33422,7 @@
       <c r="M1" s="734"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="668"/>
+      <c r="B2" s="692"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -33417,21 +33432,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="671" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="672"/>
+      <c r="B3" s="695" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="696"/>
       <c r="D3" s="10"/>
       <c r="E3" s="556"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="673" t="s">
+      <c r="H3" s="697" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="673"/>
+      <c r="I3" s="697"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="710" t="s">
+      <c r="P3" s="721" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="731" t="s">
@@ -33453,14 +33468,14 @@
       <c r="D4" s="18">
         <v>44710</v>
       </c>
-      <c r="E4" s="674" t="s">
+      <c r="E4" s="698" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="675"/>
-      <c r="H4" s="676" t="s">
+      <c r="F4" s="699"/>
+      <c r="H4" s="700" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="677"/>
+      <c r="I4" s="701"/>
       <c r="J4" s="559"/>
       <c r="K4" s="565"/>
       <c r="L4" s="566"/>
@@ -33470,15 +33485,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="711"/>
+      <c r="P4" s="722"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="732"/>
       <c r="U4" s="34"/>
       <c r="V4" s="128"/>
-      <c r="W4" s="793"/>
-      <c r="X4" s="793"/>
+      <c r="W4" s="796"/>
+      <c r="X4" s="796"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -33533,8 +33548,8 @@
       <c r="S5" s="324"/>
       <c r="U5" s="34"/>
       <c r="V5" s="128"/>
-      <c r="W5" s="793"/>
-      <c r="X5" s="793"/>
+      <c r="W5" s="796"/>
+      <c r="X5" s="796"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -34310,7 +34325,7 @@
       <c r="S19" s="147"/>
       <c r="U19" s="34"/>
       <c r="V19" s="128"/>
-      <c r="W19" s="794"/>
+      <c r="W19" s="797"/>
       <c r="X19" s="544"/>
       <c r="Y19" s="233"/>
     </row>
@@ -34364,7 +34379,7 @@
       <c r="S20" s="147"/>
       <c r="U20" s="34"/>
       <c r="V20" s="128"/>
-      <c r="W20" s="794"/>
+      <c r="W20" s="797"/>
       <c r="X20" s="34"/>
       <c r="Y20" s="233"/>
     </row>
@@ -34373,29 +34388,40 @@
       <c r="B21" s="24">
         <v>44727</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="35"/>
+      <c r="C21" s="25">
+        <v>20445</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>934</v>
+      </c>
       <c r="E21" s="27">
         <v>44727</v>
       </c>
-      <c r="F21" s="28"/>
+      <c r="F21" s="28">
+        <v>104472</v>
+      </c>
       <c r="G21" s="575"/>
       <c r="H21" s="29">
         <v>44727</v>
       </c>
-      <c r="I21" s="30"/>
+      <c r="I21" s="30">
+        <v>3516.5</v>
+      </c>
       <c r="J21" s="37"/>
       <c r="K21" s="568"/>
       <c r="L21" s="45"/>
       <c r="M21" s="32">
-        <v>0</v>
+        <v>36290.5</v>
       </c>
       <c r="N21" s="33">
-        <v>0</v>
+        <v>44220</v>
+      </c>
+      <c r="O21" s="663" t="s">
+        <v>917</v>
       </c>
       <c r="P21" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>104472</v>
       </c>
       <c r="Q21" s="325">
         <f t="shared" si="0"/>
@@ -34407,8 +34433,8 @@
       <c r="S21" s="147"/>
       <c r="U21" s="34"/>
       <c r="V21" s="128"/>
-      <c r="W21" s="726"/>
-      <c r="X21" s="726"/>
+      <c r="W21" s="710"/>
+      <c r="X21" s="710"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -34417,29 +34443,40 @@
       <c r="B22" s="24">
         <v>44728</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="35"/>
+      <c r="C22" s="25">
+        <v>15995</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>935</v>
+      </c>
       <c r="E22" s="27">
         <v>44728</v>
       </c>
-      <c r="F22" s="28"/>
+      <c r="F22" s="28">
+        <v>120324</v>
+      </c>
       <c r="G22" s="575"/>
       <c r="H22" s="29">
         <v>44728</v>
       </c>
-      <c r="I22" s="30"/>
+      <c r="I22" s="30">
+        <v>1076</v>
+      </c>
       <c r="J22" s="37"/>
       <c r="K22" s="31"/>
       <c r="L22" s="49"/>
       <c r="M22" s="32">
-        <v>0</v>
+        <v>49576</v>
       </c>
       <c r="N22" s="33">
-        <v>0</v>
+        <v>53677</v>
+      </c>
+      <c r="O22" s="663" t="s">
+        <v>917</v>
       </c>
       <c r="P22" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>120324</v>
       </c>
       <c r="Q22" s="325">
         <f t="shared" si="0"/>
@@ -34461,29 +34498,40 @@
       <c r="B23" s="24">
         <v>44729</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="35"/>
+      <c r="C23" s="25">
+        <v>22532</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>936</v>
+      </c>
       <c r="E23" s="27">
         <v>44729</v>
       </c>
-      <c r="F23" s="28"/>
+      <c r="F23" s="28">
+        <v>114878</v>
+      </c>
       <c r="G23" s="575"/>
       <c r="H23" s="29">
         <v>44729</v>
       </c>
-      <c r="I23" s="30"/>
+      <c r="I23" s="30">
+        <v>3793</v>
+      </c>
       <c r="J23" s="50"/>
       <c r="K23" s="172"/>
       <c r="L23" s="45"/>
       <c r="M23" s="32">
-        <v>0</v>
+        <v>48123</v>
       </c>
       <c r="N23" s="33">
-        <v>0</v>
+        <v>40430</v>
+      </c>
+      <c r="O23" s="663" t="s">
+        <v>917</v>
       </c>
       <c r="P23" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>114878</v>
       </c>
       <c r="Q23" s="325">
         <f t="shared" si="0"/>
@@ -34495,8 +34543,8 @@
       <c r="S23" s="147"/>
       <c r="U23" s="34"/>
       <c r="V23" s="128"/>
-      <c r="W23" s="727"/>
-      <c r="X23" s="727"/>
+      <c r="W23" s="711"/>
+      <c r="X23" s="711"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -34505,33 +34553,50 @@
       <c r="B24" s="24">
         <v>44730</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="42"/>
+      <c r="C24" s="25">
+        <v>10538</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>937</v>
+      </c>
       <c r="E24" s="27">
         <v>44730</v>
       </c>
-      <c r="F24" s="28"/>
+      <c r="F24" s="28">
+        <v>170128</v>
+      </c>
       <c r="G24" s="575"/>
       <c r="H24" s="29">
         <v>44730</v>
       </c>
-      <c r="I24" s="30"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="173"/>
-      <c r="L24" s="52"/>
+      <c r="I24" s="30">
+        <v>4444</v>
+      </c>
+      <c r="J24" s="51">
+        <v>44730</v>
+      </c>
+      <c r="K24" s="173" t="s">
+        <v>938</v>
+      </c>
+      <c r="L24" s="52">
+        <v>17514</v>
+      </c>
       <c r="M24" s="32">
-        <v>0</v>
+        <v>66300</v>
       </c>
       <c r="N24" s="33">
-        <v>0</v>
+        <v>71337</v>
+      </c>
+      <c r="O24" s="663" t="s">
+        <v>917</v>
       </c>
       <c r="P24" s="39">
         <f>N24+M24+L24+I24+C24</f>
-        <v>0</v>
+        <v>170133</v>
       </c>
       <c r="Q24" s="325">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R24" s="319">
         <v>0</v>
@@ -34539,8 +34604,8 @@
       <c r="S24" s="147"/>
       <c r="U24" s="34"/>
       <c r="V24" s="128"/>
-      <c r="W24" s="727"/>
-      <c r="X24" s="727"/>
+      <c r="W24" s="711"/>
+      <c r="X24" s="711"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -34582,8 +34647,8 @@
       </c>
       <c r="U25" s="34"/>
       <c r="V25" s="128"/>
-      <c r="W25" s="728"/>
-      <c r="X25" s="728"/>
+      <c r="W25" s="712"/>
+      <c r="X25" s="712"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -34627,8 +34692,8 @@
       <c r="T26" s="128"/>
       <c r="U26" s="34"/>
       <c r="V26" s="128"/>
-      <c r="W26" s="728"/>
-      <c r="X26" s="728"/>
+      <c r="W26" s="712"/>
+      <c r="X26" s="712"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -34672,9 +34737,9 @@
       <c r="T27" s="128"/>
       <c r="U27" s="34"/>
       <c r="V27" s="128"/>
-      <c r="W27" s="721"/>
-      <c r="X27" s="722"/>
-      <c r="Y27" s="723"/>
+      <c r="W27" s="705"/>
+      <c r="X27" s="706"/>
+      <c r="Y27" s="707"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -34717,9 +34782,9 @@
       <c r="T28" s="128"/>
       <c r="U28" s="34"/>
       <c r="V28" s="128"/>
-      <c r="W28" s="722"/>
-      <c r="X28" s="722"/>
-      <c r="Y28" s="723"/>
+      <c r="W28" s="706"/>
+      <c r="X28" s="706"/>
+      <c r="Y28" s="707"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -35243,21 +35308,21 @@
       <c r="L41" s="39">
         <v>18992.37</v>
       </c>
-      <c r="M41" s="712">
+      <c r="M41" s="723">
         <f>SUM(M5:M40)</f>
-        <v>756320</v>
-      </c>
-      <c r="N41" s="712">
+        <v>956609.5</v>
+      </c>
+      <c r="N41" s="723">
         <f>SUM(N5:N40)</f>
-        <v>573705</v>
+        <v>783369</v>
       </c>
       <c r="P41" s="506">
         <f>SUM(P5:P40)</f>
-        <v>1666314.55</v>
+        <v>2176121.5499999998</v>
       </c>
       <c r="Q41" s="771">
         <f>SUM(Q5:Q40)</f>
-        <v>25.55000000000291</v>
+        <v>30.55000000000291</v>
       </c>
     </row>
     <row r="42" spans="1:24" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -35279,8 +35344,8 @@
       <c r="L42" s="52">
         <v>17035.3</v>
       </c>
-      <c r="M42" s="713"/>
-      <c r="N42" s="713"/>
+      <c r="M42" s="724"/>
+      <c r="N42" s="724"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="772"/>
     </row>
@@ -35294,9 +35359,15 @@
       <c r="G43" s="575"/>
       <c r="H43" s="76"/>
       <c r="I43" s="77"/>
-      <c r="J43" s="50"/>
-      <c r="K43" s="38"/>
-      <c r="L43" s="54"/>
+      <c r="J43" s="50">
+        <v>44730</v>
+      </c>
+      <c r="K43" s="38" t="s">
+        <v>938</v>
+      </c>
+      <c r="L43" s="54">
+        <v>18951.07</v>
+      </c>
       <c r="M43" s="648"/>
       <c r="N43" s="648"/>
       <c r="P43" s="34"/>
@@ -35335,7 +35406,7 @@
       <c r="L45" s="39"/>
       <c r="M45" s="773">
         <f>M41+N41</f>
-        <v>1330025</v>
+        <v>1739978.5</v>
       </c>
       <c r="N45" s="774"/>
       <c r="P45" s="34"/>
@@ -35618,7 +35689,7 @@
       </c>
       <c r="C61" s="87">
         <f>SUM(C5:C60)</f>
-        <v>255189</v>
+        <v>324699</v>
       </c>
       <c r="D61" s="88"/>
       <c r="E61" s="91" t="s">
@@ -35626,7 +35697,7 @@
       </c>
       <c r="F61" s="90">
         <f>SUM(F5:F60)</f>
-        <v>1637524</v>
+        <v>2147326</v>
       </c>
       <c r="G61" s="576"/>
       <c r="H61" s="91" t="s">
@@ -35634,7 +35705,7 @@
       </c>
       <c r="I61" s="92">
         <f>SUM(I5:I60)</f>
-        <v>45556</v>
+        <v>58385.5</v>
       </c>
       <c r="J61" s="93"/>
       <c r="K61" s="94" t="s">
@@ -35642,7 +35713,7 @@
       </c>
       <c r="L61" s="95">
         <f>SUM(L5:L60)</f>
-        <v>71572.22</v>
+        <v>108037.29000000001</v>
       </c>
       <c r="M61" s="96"/>
       <c r="N61" s="96"/>
@@ -35660,50 +35731,50 @@
       <c r="A63" s="98"/>
       <c r="B63" s="99"/>
       <c r="C63" s="1"/>
-      <c r="H63" s="689" t="s">
+      <c r="H63" s="678" t="s">
         <v>11</v>
       </c>
-      <c r="I63" s="690"/>
+      <c r="I63" s="679"/>
       <c r="J63" s="562"/>
-      <c r="K63" s="796">
+      <c r="K63" s="793">
         <f>I61+L61</f>
-        <v>117128.22</v>
-      </c>
-      <c r="L63" s="797"/>
+        <v>166422.79</v>
+      </c>
+      <c r="L63" s="794"/>
       <c r="M63" s="272"/>
       <c r="N63" s="272"/>
       <c r="P63" s="34"/>
       <c r="Q63" s="13"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D64" s="695" t="s">
+      <c r="D64" s="684" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="695"/>
+      <c r="E64" s="684"/>
       <c r="F64" s="312">
         <f>F61-K63-C61</f>
-        <v>1265206.78</v>
+        <v>1656204.21</v>
       </c>
       <c r="I64" s="102"/>
       <c r="J64" s="563"/>
     </row>
     <row r="65" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D65" s="719" t="s">
+      <c r="D65" s="714" t="s">
         <v>95</v>
       </c>
-      <c r="E65" s="719"/>
+      <c r="E65" s="714"/>
       <c r="F65" s="111">
         <v>0</v>
       </c>
-      <c r="I65" s="696" t="s">
+      <c r="I65" s="685" t="s">
         <v>13</v>
       </c>
-      <c r="J65" s="697"/>
-      <c r="K65" s="698">
+      <c r="J65" s="686"/>
+      <c r="K65" s="687">
         <f>F67+F68+F69</f>
-        <v>1265206.78</v>
-      </c>
-      <c r="L65" s="698"/>
+        <v>1656204.21</v>
+      </c>
+      <c r="L65" s="687"/>
       <c r="M65" s="404"/>
       <c r="N65" s="404"/>
       <c r="O65" s="660"/>
@@ -35737,7 +35808,7 @@
       </c>
       <c r="F67" s="96">
         <f>SUM(F64:F66)</f>
-        <v>1265206.78</v>
+        <v>1656204.21</v>
       </c>
       <c r="H67" s="558"/>
       <c r="I67" s="108" t="s">
@@ -35748,7 +35819,7 @@
         <f>-C4</f>
         <v>-2546982.16</v>
       </c>
-      <c r="L67" s="698"/>
+      <c r="L67" s="687"/>
     </row>
     <row r="68" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="110" t="s">
@@ -35763,22 +35834,22 @@
     </row>
     <row r="69" spans="2:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C69" s="112"/>
-      <c r="D69" s="678" t="s">
+      <c r="D69" s="667" t="s">
         <v>18</v>
       </c>
-      <c r="E69" s="679"/>
+      <c r="E69" s="668"/>
       <c r="F69" s="113">
         <v>0</v>
       </c>
-      <c r="I69" s="680" t="s">
+      <c r="I69" s="669" t="s">
         <v>198</v>
       </c>
-      <c r="J69" s="681"/>
-      <c r="K69" s="682">
+      <c r="J69" s="670"/>
+      <c r="K69" s="671">
         <f>K65+K67</f>
-        <v>-1281775.3800000001</v>
-      </c>
-      <c r="L69" s="682"/>
+        <v>-890777.95000000019</v>
+      </c>
+      <c r="L69" s="671"/>
     </row>
     <row r="70" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C70" s="114"/>
@@ -35922,6 +35993,26 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="K67:L67"/>
     <mergeCell ref="D69:E69"/>
     <mergeCell ref="I69:J69"/>
     <mergeCell ref="K69:L69"/>
@@ -35932,26 +36023,6 @@
     <mergeCell ref="D65:E65"/>
     <mergeCell ref="I65:J65"/>
     <mergeCell ref="K65:L65"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="K67:L67"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -41124,23 +41195,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="667"/>
-      <c r="C1" s="669" t="s">
+      <c r="B1" s="691"/>
+      <c r="C1" s="693" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="670"/>
-      <c r="E1" s="670"/>
-      <c r="F1" s="670"/>
-      <c r="G1" s="670"/>
-      <c r="H1" s="670"/>
-      <c r="I1" s="670"/>
-      <c r="J1" s="670"/>
-      <c r="K1" s="670"/>
-      <c r="L1" s="670"/>
-      <c r="M1" s="670"/>
+      <c r="D1" s="694"/>
+      <c r="E1" s="694"/>
+      <c r="F1" s="694"/>
+      <c r="G1" s="694"/>
+      <c r="H1" s="694"/>
+      <c r="I1" s="694"/>
+      <c r="J1" s="694"/>
+      <c r="K1" s="694"/>
+      <c r="L1" s="694"/>
+      <c r="M1" s="694"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="668"/>
+      <c r="B2" s="692"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -41150,21 +41221,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="671" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="672"/>
+      <c r="B3" s="695" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="696"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="673" t="s">
+      <c r="H3" s="697" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="673"/>
+      <c r="I3" s="697"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="710" t="s">
+      <c r="P3" s="721" t="s">
         <v>6</v>
       </c>
     </row>
@@ -41179,14 +41250,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="674" t="s">
+      <c r="E4" s="698" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="675"/>
-      <c r="H4" s="676" t="s">
+      <c r="F4" s="699"/>
+      <c r="H4" s="700" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="677"/>
+      <c r="I4" s="701"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -41196,14 +41267,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="711"/>
+      <c r="P4" s="722"/>
       <c r="Q4" s="286" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="720" t="s">
+      <c r="W4" s="704" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="720"/>
+      <c r="X4" s="704"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -41254,8 +41325,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="720"/>
-      <c r="X5" s="720"/>
+      <c r="W5" s="704"/>
+      <c r="X5" s="704"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -42026,7 +42097,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="724">
+      <c r="W19" s="708">
         <f>SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -42078,7 +42149,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="725"/>
+      <c r="W20" s="709"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -42127,8 +42198,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="726"/>
-      <c r="X21" s="726"/>
+      <c r="W21" s="710"/>
+      <c r="X21" s="710"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -42229,8 +42300,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="727"/>
-      <c r="X23" s="727"/>
+      <c r="W23" s="711"/>
+      <c r="X23" s="711"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -42284,8 +42355,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="727"/>
-      <c r="X24" s="727"/>
+      <c r="W24" s="711"/>
+      <c r="X24" s="711"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -42331,8 +42402,8 @@
       <c r="R25" s="285">
         <v>28952</v>
       </c>
-      <c r="W25" s="728"/>
-      <c r="X25" s="728"/>
+      <c r="W25" s="712"/>
+      <c r="X25" s="712"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -42383,8 +42454,8 @@
       <c r="R26" s="285">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="728"/>
-      <c r="X26" s="728"/>
+      <c r="W26" s="712"/>
+      <c r="X26" s="712"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -42432,9 +42503,9 @@
       <c r="R27" s="285">
         <v>14637</v>
       </c>
-      <c r="W27" s="721"/>
-      <c r="X27" s="722"/>
-      <c r="Y27" s="723"/>
+      <c r="W27" s="705"/>
+      <c r="X27" s="706"/>
+      <c r="Y27" s="707"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -42484,9 +42555,9 @@
       <c r="R28" s="285">
         <v>0</v>
       </c>
-      <c r="W28" s="722"/>
-      <c r="X28" s="722"/>
-      <c r="Y28" s="723"/>
+      <c r="W28" s="706"/>
+      <c r="X28" s="706"/>
+      <c r="Y28" s="707"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -42821,11 +42892,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="712">
+      <c r="M36" s="723">
         <f>SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="714">
+      <c r="N36" s="725">
         <f>SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -42833,7 +42904,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="716">
+      <c r="Q36" s="727">
         <f>SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -42868,13 +42939,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="713"/>
-      <c r="N37" s="715"/>
+      <c r="M37" s="724"/>
+      <c r="N37" s="726"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="717"/>
+      <c r="Q37" s="728"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -43164,26 +43235,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="689" t="s">
+      <c r="H52" s="678" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="690"/>
+      <c r="I52" s="679"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="691">
+      <c r="K52" s="680">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="718"/>
+      <c r="L52" s="713"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="695" t="s">
+      <c r="D53" s="684" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="695"/>
+      <c r="E53" s="684"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -43192,29 +43263,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="719" t="s">
+      <c r="D54" s="714" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="719"/>
+      <c r="E54" s="714"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="696" t="s">
+      <c r="I54" s="685" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="697"/>
-      <c r="K54" s="698">
+      <c r="J54" s="686"/>
+      <c r="K54" s="687">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="698"/>
-      <c r="M54" s="704" t="s">
+      <c r="L54" s="687"/>
+      <c r="M54" s="715" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="705"/>
-      <c r="O54" s="705"/>
-      <c r="P54" s="705"/>
-      <c r="Q54" s="706"/>
+      <c r="N54" s="716"/>
+      <c r="O54" s="716"/>
+      <c r="P54" s="716"/>
+      <c r="Q54" s="717"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -43228,11 +43299,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="707"/>
-      <c r="N55" s="708"/>
-      <c r="O55" s="708"/>
-      <c r="P55" s="708"/>
-      <c r="Q55" s="709"/>
+      <c r="M55" s="718"/>
+      <c r="N55" s="719"/>
+      <c r="O55" s="719"/>
+      <c r="P55" s="719"/>
+      <c r="Q55" s="720"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -43250,11 +43321,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="700">
+      <c r="K56" s="689">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="701"/>
+      <c r="L56" s="690"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -43271,22 +43342,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="678" t="s">
+      <c r="D58" s="667" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="679"/>
+      <c r="E58" s="668"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="680" t="s">
+      <c r="I58" s="669" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="681"/>
-      <c r="K58" s="682">
+      <c r="J58" s="670"/>
+      <c r="K58" s="671">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="682"/>
+      <c r="L58" s="671"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -43430,14 +43501,17 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -43448,17 +43522,14 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.27559055118110237" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="68" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -46201,23 +46272,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="667"/>
-      <c r="C1" s="669" t="s">
+      <c r="B1" s="691"/>
+      <c r="C1" s="693" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="670"/>
-      <c r="E1" s="670"/>
-      <c r="F1" s="670"/>
-      <c r="G1" s="670"/>
-      <c r="H1" s="670"/>
-      <c r="I1" s="670"/>
-      <c r="J1" s="670"/>
-      <c r="K1" s="670"/>
-      <c r="L1" s="670"/>
-      <c r="M1" s="670"/>
+      <c r="D1" s="694"/>
+      <c r="E1" s="694"/>
+      <c r="F1" s="694"/>
+      <c r="G1" s="694"/>
+      <c r="H1" s="694"/>
+      <c r="I1" s="694"/>
+      <c r="J1" s="694"/>
+      <c r="K1" s="694"/>
+      <c r="L1" s="694"/>
+      <c r="M1" s="694"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="668"/>
+      <c r="B2" s="692"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -46227,21 +46298,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="671" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="672"/>
+      <c r="B3" s="695" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="696"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="673" t="s">
+      <c r="H3" s="697" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="673"/>
+      <c r="I3" s="697"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="710" t="s">
+      <c r="P3" s="721" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="731" t="s">
@@ -46259,14 +46330,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="674" t="s">
+      <c r="E4" s="698" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="675"/>
-      <c r="H4" s="676" t="s">
+      <c r="F4" s="699"/>
+      <c r="H4" s="700" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="677"/>
+      <c r="I4" s="701"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -46276,15 +46347,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="711"/>
+      <c r="P4" s="722"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="732"/>
-      <c r="W4" s="720" t="s">
+      <c r="W4" s="704" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="720"/>
+      <c r="X4" s="704"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -46345,8 +46416,8 @@
       <c r="S5" s="324" t="s">
         <v>213</v>
       </c>
-      <c r="W5" s="720"/>
-      <c r="X5" s="720"/>
+      <c r="W5" s="704"/>
+      <c r="X5" s="704"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -47103,7 +47174,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="724">
+      <c r="W19" s="708">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -47155,7 +47226,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="725"/>
+      <c r="W20" s="709"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -47204,8 +47275,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="726"/>
-      <c r="X21" s="726"/>
+      <c r="W21" s="710"/>
+      <c r="X21" s="710"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -47306,8 +47377,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="727"/>
-      <c r="X23" s="727"/>
+      <c r="W23" s="711"/>
+      <c r="X23" s="711"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -47358,8 +47429,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="727"/>
-      <c r="X24" s="727"/>
+      <c r="W24" s="711"/>
+      <c r="X24" s="711"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -47405,8 +47476,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="728"/>
-      <c r="X25" s="728"/>
+      <c r="W25" s="712"/>
+      <c r="X25" s="712"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -47454,8 +47525,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="728"/>
-      <c r="X26" s="728"/>
+      <c r="W26" s="712"/>
+      <c r="X26" s="712"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -47515,9 +47586,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="721"/>
-      <c r="X27" s="722"/>
-      <c r="Y27" s="723"/>
+      <c r="W27" s="705"/>
+      <c r="X27" s="706"/>
+      <c r="Y27" s="707"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -47571,9 +47642,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="722"/>
-      <c r="X28" s="722"/>
-      <c r="Y28" s="723"/>
+      <c r="W28" s="706"/>
+      <c r="X28" s="706"/>
+      <c r="Y28" s="707"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -47889,11 +47960,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="712">
+      <c r="M36" s="723">
         <f>SUM(M5:M35)</f>
         <v>1077791.3</v>
       </c>
-      <c r="N36" s="714">
+      <c r="N36" s="725">
         <f>SUM(N5:N35)</f>
         <v>936398</v>
       </c>
@@ -47901,7 +47972,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="716">
+      <c r="Q36" s="727">
         <f>SUM(Q5:Q35)</f>
         <v>-14262.940000000002</v>
       </c>
@@ -47920,13 +47991,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="713"/>
-      <c r="N37" s="715"/>
+      <c r="M37" s="724"/>
+      <c r="N37" s="726"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="717"/>
+      <c r="Q37" s="728"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -48200,26 +48271,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="689" t="s">
+      <c r="H52" s="678" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="690"/>
+      <c r="I52" s="679"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="691">
+      <c r="K52" s="680">
         <f>I50+L50</f>
         <v>90750.75</v>
       </c>
-      <c r="L52" s="718"/>
+      <c r="L52" s="713"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="695" t="s">
+      <c r="D53" s="684" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="695"/>
+      <c r="E53" s="684"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>1739855.03</v>
@@ -48228,29 +48299,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="719" t="s">
+      <c r="D54" s="714" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="719"/>
+      <c r="E54" s="714"/>
       <c r="F54" s="111">
         <v>-1567070.66</v>
       </c>
-      <c r="I54" s="696" t="s">
+      <c r="I54" s="685" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="697"/>
-      <c r="K54" s="698">
+      <c r="J54" s="686"/>
+      <c r="K54" s="687">
         <f>F56+F57+F58</f>
         <v>703192.8600000001</v>
       </c>
-      <c r="L54" s="698"/>
-      <c r="M54" s="704" t="s">
+      <c r="L54" s="687"/>
+      <c r="M54" s="715" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="705"/>
-      <c r="O54" s="705"/>
-      <c r="P54" s="705"/>
-      <c r="Q54" s="706"/>
+      <c r="N54" s="716"/>
+      <c r="O54" s="716"/>
+      <c r="P54" s="716"/>
+      <c r="Q54" s="717"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -48264,11 +48335,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="707"/>
-      <c r="N55" s="708"/>
-      <c r="O55" s="708"/>
-      <c r="P55" s="708"/>
-      <c r="Q55" s="709"/>
+      <c r="M55" s="718"/>
+      <c r="N55" s="719"/>
+      <c r="O55" s="719"/>
+      <c r="P55" s="719"/>
+      <c r="Q55" s="720"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -48286,11 +48357,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="700">
+      <c r="K56" s="689">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="701"/>
+      <c r="L56" s="690"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -48307,22 +48378,22 @@
       <c r="C58" s="112">
         <v>44563</v>
       </c>
-      <c r="D58" s="678" t="s">
+      <c r="D58" s="667" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="679"/>
+      <c r="E58" s="668"/>
       <c r="F58" s="113">
         <v>754143.23</v>
       </c>
-      <c r="I58" s="680" t="s">
+      <c r="I58" s="669" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="681"/>
-      <c r="K58" s="682">
+      <c r="J58" s="670"/>
+      <c r="K58" s="671">
         <f>K54+K56</f>
         <v>135803.51000000013</v>
       </c>
-      <c r="L58" s="682"/>
+      <c r="L58" s="671"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -48466,20 +48537,13 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="H52:I52"/>
     <mergeCell ref="K52:L52"/>
     <mergeCell ref="W4:X5"/>
@@ -48489,13 +48553,20 @@
     <mergeCell ref="W25:X25"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -51190,7 +51261,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="667"/>
+      <c r="B1" s="691"/>
       <c r="C1" s="733" t="s">
         <v>316</v>
       </c>
@@ -51206,7 +51277,7 @@
       <c r="M1" s="734"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="668"/>
+      <c r="B2" s="692"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -51216,21 +51287,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="671" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="672"/>
+      <c r="B3" s="695" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="696"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="673" t="s">
+      <c r="H3" s="697" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="673"/>
+      <c r="I3" s="697"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="710" t="s">
+      <c r="P3" s="721" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="731" t="s">
@@ -51248,14 +51319,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="674" t="s">
+      <c r="E4" s="698" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="675"/>
-      <c r="H4" s="676" t="s">
+      <c r="F4" s="699"/>
+      <c r="H4" s="700" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="677"/>
+      <c r="I4" s="701"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -51265,15 +51336,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="711"/>
+      <c r="P4" s="722"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="732"/>
-      <c r="W4" s="720" t="s">
+      <c r="W4" s="704" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="720"/>
+      <c r="X4" s="704"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -51324,8 +51395,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="720"/>
-      <c r="X5" s="720"/>
+      <c r="W5" s="704"/>
+      <c r="X5" s="704"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -52089,7 +52160,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="724">
+      <c r="W19" s="708">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -52142,7 +52213,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="725"/>
+      <c r="W20" s="709"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -52191,8 +52262,8 @@
         <v>377273.87</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="726"/>
-      <c r="X21" s="726"/>
+      <c r="W21" s="710"/>
+      <c r="X21" s="710"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -52292,8 +52363,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="727"/>
-      <c r="X23" s="727"/>
+      <c r="W23" s="711"/>
+      <c r="X23" s="711"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -52348,8 +52419,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="727"/>
-      <c r="X24" s="727"/>
+      <c r="W24" s="711"/>
+      <c r="X24" s="711"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -52394,8 +52465,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="728"/>
-      <c r="X25" s="728"/>
+      <c r="W25" s="712"/>
+      <c r="X25" s="712"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -52443,8 +52514,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="728"/>
-      <c r="X26" s="728"/>
+      <c r="W26" s="712"/>
+      <c r="X26" s="712"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -52498,9 +52569,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="721"/>
-      <c r="X27" s="722"/>
-      <c r="Y27" s="723"/>
+      <c r="W27" s="705"/>
+      <c r="X27" s="706"/>
+      <c r="Y27" s="707"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -52554,9 +52625,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="722"/>
-      <c r="X28" s="722"/>
-      <c r="Y28" s="723"/>
+      <c r="W28" s="706"/>
+      <c r="X28" s="706"/>
+      <c r="Y28" s="707"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -52867,11 +52938,11 @@
       <c r="L36" s="44">
         <v>13275.84</v>
       </c>
-      <c r="M36" s="712">
+      <c r="M36" s="723">
         <f>SUM(M5:M35)</f>
         <v>1818445.73</v>
       </c>
-      <c r="N36" s="714">
+      <c r="N36" s="725">
         <f>SUM(N5:N35)</f>
         <v>739014</v>
       </c>
@@ -52879,7 +52950,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="716">
+      <c r="Q36" s="727">
         <f>SUM(Q5:Q35)</f>
         <v>-7.2800000000133878</v>
       </c>
@@ -52904,13 +52975,13 @@
       <c r="L37" s="61">
         <v>15060.32</v>
       </c>
-      <c r="M37" s="713"/>
-      <c r="N37" s="715"/>
+      <c r="M37" s="724"/>
+      <c r="N37" s="726"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="717"/>
+      <c r="Q37" s="728"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -53203,26 +53274,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="689" t="s">
+      <c r="H52" s="678" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="690"/>
+      <c r="I52" s="679"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="691">
+      <c r="K52" s="680">
         <f>I50+L50</f>
         <v>158798.12</v>
       </c>
-      <c r="L52" s="718"/>
+      <c r="L52" s="713"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="695" t="s">
+      <c r="D53" s="684" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="695"/>
+      <c r="E53" s="684"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2078470.75</v>
@@ -53231,22 +53302,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="719" t="s">
+      <c r="D54" s="714" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="719"/>
+      <c r="E54" s="714"/>
       <c r="F54" s="111">
         <v>-1448401.2</v>
       </c>
-      <c r="I54" s="696" t="s">
+      <c r="I54" s="685" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="697"/>
-      <c r="K54" s="698">
+      <c r="J54" s="686"/>
+      <c r="K54" s="687">
         <f>F56+F57+F58</f>
         <v>1025960.7</v>
       </c>
-      <c r="L54" s="698"/>
+      <c r="L54" s="687"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -53287,11 +53358,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="700">
+      <c r="K56" s="689">
         <f>-C4</f>
         <v>-754143.23</v>
       </c>
-      <c r="L56" s="701"/>
+      <c r="L56" s="690"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -53308,22 +53379,22 @@
       <c r="C58" s="112">
         <v>44591</v>
       </c>
-      <c r="D58" s="678" t="s">
+      <c r="D58" s="667" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="679"/>
+      <c r="E58" s="668"/>
       <c r="F58" s="113">
         <v>1149740.4099999999</v>
       </c>
-      <c r="I58" s="680" t="s">
+      <c r="I58" s="669" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="681"/>
-      <c r="K58" s="682">
+      <c r="J58" s="670"/>
+      <c r="K58" s="671">
         <f>K54+K56</f>
         <v>271817.46999999997</v>
       </c>
-      <c r="L58" s="682"/>
+      <c r="L58" s="671"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -53467,20 +53538,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="K52:L52"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -53496,6 +53553,20 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="K52:L52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -56289,7 +56360,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="667"/>
+      <c r="B1" s="691"/>
       <c r="C1" s="733" t="s">
         <v>646</v>
       </c>
@@ -56305,7 +56376,7 @@
       <c r="M1" s="734"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="668"/>
+      <c r="B2" s="692"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -56315,21 +56386,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="671" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="672"/>
+      <c r="B3" s="695" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="696"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="673" t="s">
+      <c r="H3" s="697" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="673"/>
+      <c r="I3" s="697"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="710" t="s">
+      <c r="P3" s="721" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="731" t="s">
@@ -56347,14 +56418,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="674" t="s">
+      <c r="E4" s="698" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="675"/>
-      <c r="H4" s="676" t="s">
+      <c r="F4" s="699"/>
+      <c r="H4" s="700" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="677"/>
+      <c r="I4" s="701"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -56364,15 +56435,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="711"/>
+      <c r="P4" s="722"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="732"/>
-      <c r="W4" s="720" t="s">
+      <c r="W4" s="704" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="720"/>
+      <c r="X4" s="704"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -56423,8 +56494,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="720"/>
-      <c r="X5" s="720"/>
+      <c r="W5" s="704"/>
+      <c r="X5" s="704"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -57185,7 +57256,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="724">
+      <c r="W19" s="708">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -57237,7 +57308,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="725"/>
+      <c r="W20" s="709"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -57286,8 +57357,8 @@
         <v>18072</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="726"/>
-      <c r="X21" s="726"/>
+      <c r="W21" s="710"/>
+      <c r="X21" s="710"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -57386,8 +57457,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="727"/>
-      <c r="X23" s="727"/>
+      <c r="W23" s="711"/>
+      <c r="X23" s="711"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -57442,8 +57513,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="727"/>
-      <c r="X24" s="727"/>
+      <c r="W24" s="711"/>
+      <c r="X24" s="711"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -57491,8 +57562,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="728"/>
-      <c r="X25" s="728"/>
+      <c r="W25" s="712"/>
+      <c r="X25" s="712"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -57540,8 +57611,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="728"/>
-      <c r="X26" s="728"/>
+      <c r="W26" s="712"/>
+      <c r="X26" s="712"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -57589,9 +57660,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="721"/>
-      <c r="X27" s="722"/>
-      <c r="Y27" s="723"/>
+      <c r="W27" s="705"/>
+      <c r="X27" s="706"/>
+      <c r="Y27" s="707"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -57639,9 +57710,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="722"/>
-      <c r="X28" s="722"/>
-      <c r="Y28" s="723"/>
+      <c r="W28" s="706"/>
+      <c r="X28" s="706"/>
+      <c r="Y28" s="707"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -57982,11 +58053,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="712">
+      <c r="M36" s="723">
         <f>SUM(M5:M35)</f>
         <v>2143864.4900000002</v>
       </c>
-      <c r="N36" s="714">
+      <c r="N36" s="725">
         <f>SUM(N5:N35)</f>
         <v>791108</v>
       </c>
@@ -58019,8 +58090,8 @@
       <c r="L37" s="61">
         <v>16518.78</v>
       </c>
-      <c r="M37" s="713"/>
-      <c r="N37" s="715"/>
+      <c r="M37" s="724"/>
+      <c r="N37" s="726"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
@@ -58327,26 +58398,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="689" t="s">
+      <c r="H52" s="678" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="690"/>
+      <c r="I52" s="679"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="691">
+      <c r="K52" s="680">
         <f>I50+L50</f>
         <v>197471.8</v>
       </c>
-      <c r="L52" s="718"/>
+      <c r="L52" s="713"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="695" t="s">
+      <c r="D53" s="684" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="695"/>
+      <c r="E53" s="684"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2057786.11</v>
@@ -58355,22 +58426,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="719" t="s">
+      <c r="D54" s="714" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="719"/>
+      <c r="E54" s="714"/>
       <c r="F54" s="111">
         <v>-1702928.14</v>
       </c>
-      <c r="I54" s="696" t="s">
+      <c r="I54" s="685" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="697"/>
-      <c r="K54" s="698">
+      <c r="J54" s="686"/>
+      <c r="K54" s="687">
         <f>F56+F57+F58</f>
         <v>1147965.3400000003</v>
       </c>
-      <c r="L54" s="698"/>
+      <c r="L54" s="687"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -58411,11 +58482,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="700">
+      <c r="K56" s="689">
         <f>-C4</f>
         <v>-1149740.4099999999</v>
       </c>
-      <c r="L56" s="701"/>
+      <c r="L56" s="690"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -58432,22 +58503,22 @@
       <c r="C58" s="112">
         <v>44619</v>
       </c>
-      <c r="D58" s="678" t="s">
+      <c r="D58" s="667" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="679"/>
+      <c r="E58" s="668"/>
       <c r="F58" s="113">
         <v>1266568.45</v>
       </c>
-      <c r="I58" s="680" t="s">
+      <c r="I58" s="669" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="681"/>
-      <c r="K58" s="682">
+      <c r="J58" s="670"/>
+      <c r="K58" s="671">
         <f>K54+K56</f>
         <v>-1775.0699999995995</v>
       </c>
-      <c r="L58" s="682"/>
+      <c r="L58" s="671"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -58591,6 +58662,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -58607,20 +58692,6 @@
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
     <mergeCell ref="M39:N39"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
   </mergeCells>
   <pageMargins left="0.23" right="0.23" top="0.4" bottom="0.28000000000000003" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 7 JUL 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/BALANCE    ZAVALETA   JUNIO    2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/BALANCE    ZAVALETA   JUNIO    2022.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROUSS\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL  ARCHIVO   2 0 2 2\CENTRAL #06  JUNIO 2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rouss\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL  ARCHIVO   2 0 2 2\CENTRAL #06  JUNIO 2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220E7BED-A2EC-4874-B961-8266C3479506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="15" activeTab="17"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OCTUBRE      2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -34,22 +35,30 @@
     <sheet name="Hoja2" sheetId="23" r:id="rId20"/>
     <sheet name="Hoja3" sheetId="20" r:id="rId21"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ROUSS</author>
   </authors>
   <commentList>
-    <comment ref="J23" authorId="0" shapeId="0">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0" shapeId="0">
+    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -102,12 +111,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ROUSS</author>
   </authors>
   <commentList>
-    <comment ref="J23" authorId="0" shapeId="0">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -131,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0" shapeId="0">
+    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -160,12 +169,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ROUSS</author>
   </authors>
   <commentList>
-    <comment ref="J23" authorId="0" shapeId="0">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -189,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0" shapeId="0">
+    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -218,12 +227,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ROUSS</author>
   </authors>
   <commentList>
-    <comment ref="J23" authorId="0" shapeId="0">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -247,7 +256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0" shapeId="0">
+    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -271,7 +280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J43" authorId="0" shapeId="0">
+    <comment ref="J43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
       <text>
         <r>
           <rPr>
@@ -300,12 +309,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ROUSS</author>
   </authors>
   <commentList>
-    <comment ref="J23" authorId="0" shapeId="0">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -329,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0" shapeId="0">
+    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
       <text>
         <r>
           <rPr>
@@ -353,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J43" authorId="0" shapeId="0">
+    <comment ref="J43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000003000000}">
       <text>
         <r>
           <rPr>
@@ -382,12 +391,12 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ROUSS</author>
   </authors>
   <commentList>
-    <comment ref="J23" authorId="0" shapeId="0">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -411,7 +420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0" shapeId="0">
+    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -435,7 +444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J43" authorId="0" shapeId="0">
+    <comment ref="J43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000003000000}">
       <text>
         <r>
           <rPr>
@@ -464,12 +473,12 @@
 </file>
 
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ROUSS</author>
   </authors>
   <commentList>
-    <comment ref="J23" authorId="0" shapeId="0">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -493,7 +502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0" shapeId="0">
+    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -517,7 +526,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J43" authorId="0" shapeId="0">
+    <comment ref="J43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000003000000}">
       <text>
         <r>
           <rPr>
@@ -546,12 +555,12 @@
 </file>
 
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ROUSS</author>
   </authors>
   <commentList>
-    <comment ref="J23" authorId="0" shapeId="0">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -575,7 +584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0" shapeId="0">
+    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -599,7 +608,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J43" authorId="0" shapeId="0">
+    <comment ref="J43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000003000000}">
       <text>
         <r>
           <rPr>
@@ -628,12 +637,12 @@
 </file>
 
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ROUSS</author>
   </authors>
   <commentList>
-    <comment ref="J23" authorId="0" shapeId="0">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -657,7 +666,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0" shapeId="0">
+    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -681,7 +690,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J43" authorId="0" shapeId="0">
+    <comment ref="J43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -3662,7 +3671,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
@@ -7072,39 +7081,6 @@
     <xf numFmtId="164" fontId="72" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7177,10 +7153,76 @@
     <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -7224,39 +7266,6 @@
     </xf>
     <xf numFmtId="44" fontId="41" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7450,20 +7459,20 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="11" fillId="18" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7961,7 +7970,7 @@
         <xdr:cNvPr id="2" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2012060D-6A0F-41D2-A832-74F72EF945FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8014,7 +8023,7 @@
         <xdr:cNvPr id="3" name="1 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C84F863B-1E69-40C9-AAA6-E150E727BC58}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8067,7 +8076,7 @@
         <xdr:cNvPr id="4" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F282856-1683-4627-996E-9F4AD530C284}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8120,7 +8129,7 @@
         <xdr:cNvPr id="5" name="Conector recto de flecha 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC19A0EA-B603-496A-8B2F-50F1F36E5D63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8173,7 +8182,7 @@
         <xdr:cNvPr id="6" name="Abrir llave 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97978218-9641-42D3-AAF9-C49E03D3CF46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8229,7 +8238,7 @@
         <xdr:cNvPr id="7" name="Rectángulo 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81AED0B7-5349-49AD-8D5B-E24B093B3905}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8329,7 +8338,7 @@
         <xdr:cNvPr id="8" name="Conector recto de flecha 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE3DEEAA-4813-4B55-9D28-E8AF250AE061}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8387,7 +8396,7 @@
         <xdr:cNvPr id="2" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2012060D-6A0F-41D2-A832-74F72EF945FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8440,7 +8449,7 @@
         <xdr:cNvPr id="3" name="1 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C84F863B-1E69-40C9-AAA6-E150E727BC58}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8493,7 +8502,7 @@
         <xdr:cNvPr id="4" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F282856-1683-4627-996E-9F4AD530C284}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8546,7 +8555,7 @@
         <xdr:cNvPr id="5" name="Conector recto de flecha 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC19A0EA-B603-496A-8B2F-50F1F36E5D63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8599,7 +8608,7 @@
         <xdr:cNvPr id="6" name="Abrir llave 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97978218-9641-42D3-AAF9-C49E03D3CF46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8655,7 +8664,7 @@
         <xdr:cNvPr id="7" name="Rectángulo 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81AED0B7-5349-49AD-8D5B-E24B093B3905}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8755,7 +8764,7 @@
         <xdr:cNvPr id="8" name="Conector recto de flecha 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE3DEEAA-4813-4B55-9D28-E8AF250AE061}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9239,7 +9248,7 @@
         <xdr:cNvPr id="2" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2012060D-6A0F-41D2-A832-74F72EF945FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9292,7 +9301,7 @@
         <xdr:cNvPr id="3" name="1 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C84F863B-1E69-40C9-AAA6-E150E727BC58}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9345,7 +9354,7 @@
         <xdr:cNvPr id="4" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F282856-1683-4627-996E-9F4AD530C284}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9398,7 +9407,7 @@
         <xdr:cNvPr id="5" name="Conector recto de flecha 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC19A0EA-B603-496A-8B2F-50F1F36E5D63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9451,7 +9460,7 @@
         <xdr:cNvPr id="6" name="Abrir llave 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97978218-9641-42D3-AAF9-C49E03D3CF46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9507,7 +9516,7 @@
         <xdr:cNvPr id="7" name="Rectángulo 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81AED0B7-5349-49AD-8D5B-E24B093B3905}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9607,7 +9616,7 @@
         <xdr:cNvPr id="8" name="Conector recto de flecha 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE3DEEAA-4813-4B55-9D28-E8AF250AE061}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9665,7 +9674,7 @@
         <xdr:cNvPr id="2" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2012060D-6A0F-41D2-A832-74F72EF945FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9718,7 +9727,7 @@
         <xdr:cNvPr id="3" name="1 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C84F863B-1E69-40C9-AAA6-E150E727BC58}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9771,7 +9780,7 @@
         <xdr:cNvPr id="4" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F282856-1683-4627-996E-9F4AD530C284}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9824,7 +9833,7 @@
         <xdr:cNvPr id="5" name="Conector recto de flecha 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC19A0EA-B603-496A-8B2F-50F1F36E5D63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9877,7 +9886,7 @@
         <xdr:cNvPr id="6" name="Abrir llave 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97978218-9641-42D3-AAF9-C49E03D3CF46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9933,7 +9942,7 @@
         <xdr:cNvPr id="7" name="Rectángulo 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81AED0B7-5349-49AD-8D5B-E24B093B3905}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10033,7 +10042,7 @@
         <xdr:cNvPr id="8" name="Conector recto de flecha 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE3DEEAA-4813-4B55-9D28-E8AF250AE061}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10088,7 +10097,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Cerrar llave 1"/>
+        <xdr:cNvPr id="2" name="Cerrar llave 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10143,7 +10158,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Cerrar llave 2"/>
+        <xdr:cNvPr id="3" name="Cerrar llave 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10206,7 +10227,7 @@
         <xdr:cNvPr id="2" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2012060D-6A0F-41D2-A832-74F72EF945FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10259,7 +10280,7 @@
         <xdr:cNvPr id="3" name="1 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C84F863B-1E69-40C9-AAA6-E150E727BC58}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10312,7 +10333,7 @@
         <xdr:cNvPr id="4" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F282856-1683-4627-996E-9F4AD530C284}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10365,7 +10386,7 @@
         <xdr:cNvPr id="5" name="Conector recto de flecha 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC19A0EA-B603-496A-8B2F-50F1F36E5D63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10418,7 +10439,7 @@
         <xdr:cNvPr id="6" name="Abrir llave 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97978218-9641-42D3-AAF9-C49E03D3CF46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10474,7 +10495,7 @@
         <xdr:cNvPr id="7" name="Rectángulo 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81AED0B7-5349-49AD-8D5B-E24B093B3905}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10574,7 +10595,7 @@
         <xdr:cNvPr id="8" name="Conector recto de flecha 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE3DEEAA-4813-4B55-9D28-E8AF250AE061}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10632,7 +10653,7 @@
         <xdr:cNvPr id="2" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2012060D-6A0F-41D2-A832-74F72EF945FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10685,7 +10706,7 @@
         <xdr:cNvPr id="3" name="1 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C84F863B-1E69-40C9-AAA6-E150E727BC58}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10738,7 +10759,7 @@
         <xdr:cNvPr id="4" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F282856-1683-4627-996E-9F4AD530C284}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10791,7 +10812,7 @@
         <xdr:cNvPr id="5" name="Conector recto de flecha 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC19A0EA-B603-496A-8B2F-50F1F36E5D63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10844,7 +10865,7 @@
         <xdr:cNvPr id="6" name="Abrir llave 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97978218-9641-42D3-AAF9-C49E03D3CF46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10900,7 +10921,7 @@
         <xdr:cNvPr id="7" name="Rectángulo 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81AED0B7-5349-49AD-8D5B-E24B093B3905}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11000,7 +11021,7 @@
         <xdr:cNvPr id="8" name="Conector recto de flecha 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE3DEEAA-4813-4B55-9D28-E8AF250AE061}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11058,7 +11079,7 @@
         <xdr:cNvPr id="2" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2012060D-6A0F-41D2-A832-74F72EF945FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11111,7 +11132,7 @@
         <xdr:cNvPr id="3" name="1 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C84F863B-1E69-40C9-AAA6-E150E727BC58}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11164,7 +11185,7 @@
         <xdr:cNvPr id="4" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F282856-1683-4627-996E-9F4AD530C284}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11217,7 +11238,7 @@
         <xdr:cNvPr id="5" name="Conector recto de flecha 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC19A0EA-B603-496A-8B2F-50F1F36E5D63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11270,7 +11291,7 @@
         <xdr:cNvPr id="6" name="Abrir llave 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97978218-9641-42D3-AAF9-C49E03D3CF46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11326,7 +11347,7 @@
         <xdr:cNvPr id="7" name="Rectángulo 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81AED0B7-5349-49AD-8D5B-E24B093B3905}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11426,7 +11447,7 @@
         <xdr:cNvPr id="8" name="Conector recto de flecha 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE3DEEAA-4813-4B55-9D28-E8AF250AE061}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11481,7 +11502,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Conector recto de flecha 2"/>
+        <xdr:cNvPr id="3" name="Conector recto de flecha 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -11529,7 +11556,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Conector recto de flecha 4"/>
+        <xdr:cNvPr id="5" name="Conector recto de flecha 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -11826,7 +11859,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF800000"/>
   </sheetPr>
@@ -11858,23 +11891,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="675"/>
-      <c r="C1" s="677" t="s">
+      <c r="B1" s="699"/>
+      <c r="C1" s="701" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="678"/>
-      <c r="E1" s="678"/>
-      <c r="F1" s="678"/>
-      <c r="G1" s="678"/>
-      <c r="H1" s="678"/>
-      <c r="I1" s="678"/>
-      <c r="J1" s="678"/>
-      <c r="K1" s="678"/>
-      <c r="L1" s="678"/>
-      <c r="M1" s="678"/>
+      <c r="D1" s="702"/>
+      <c r="E1" s="702"/>
+      <c r="F1" s="702"/>
+      <c r="G1" s="702"/>
+      <c r="H1" s="702"/>
+      <c r="I1" s="702"/>
+      <c r="J1" s="702"/>
+      <c r="K1" s="702"/>
+      <c r="L1" s="702"/>
+      <c r="M1" s="702"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="676"/>
+      <c r="B2" s="700"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -11884,17 +11917,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="679" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="680"/>
+      <c r="B3" s="703" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="704"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="681" t="s">
+      <c r="H3" s="705" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="681"/>
+      <c r="I3" s="705"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -11908,14 +11941,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="682" t="s">
+      <c r="E4" s="706" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="683"/>
-      <c r="H4" s="684" t="s">
+      <c r="F4" s="707"/>
+      <c r="H4" s="708" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="685"/>
+      <c r="I4" s="709"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -11925,10 +11958,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="691" t="s">
+      <c r="P4" s="680" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="692"/>
+      <c r="Q4" s="681"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -13369,11 +13402,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="693">
+      <c r="M39" s="682">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="695">
+      <c r="N39" s="684">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -13399,8 +13432,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="694"/>
-      <c r="N40" s="696"/>
+      <c r="M40" s="683"/>
+      <c r="N40" s="685"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -13615,29 +13648,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="697" t="s">
+      <c r="H52" s="686" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="698"/>
+      <c r="I52" s="687"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="699">
+      <c r="K52" s="688">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="700"/>
-      <c r="M52" s="701">
+      <c r="L52" s="689"/>
+      <c r="M52" s="690">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="702"/>
+      <c r="N52" s="691"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="703" t="s">
+      <c r="D53" s="692" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="703"/>
+      <c r="E53" s="692"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -13648,22 +13681,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="703" t="s">
+      <c r="D54" s="692" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="703"/>
+      <c r="E54" s="692"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="704" t="s">
+      <c r="I54" s="693" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="705"/>
-      <c r="K54" s="706">
+      <c r="J54" s="694"/>
+      <c r="K54" s="695">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="707"/>
+      <c r="L54" s="696"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -13696,11 +13729,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="708">
+      <c r="K56" s="697">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="709"/>
+      <c r="L56" s="698"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -13717,22 +13750,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="686" t="s">
+      <c r="D58" s="675" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="687"/>
+      <c r="E58" s="676"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="688" t="s">
+      <c r="I58" s="677" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="689"/>
-      <c r="K58" s="690">
+      <c r="J58" s="678"/>
+      <c r="K58" s="679">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="690"/>
+      <c r="L58" s="679"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -13876,6 +13909,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -13890,12 +13929,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -13905,7 +13938,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -16718,7 +16751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -16754,7 +16787,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="675"/>
+      <c r="B1" s="699"/>
       <c r="C1" s="741" t="s">
         <v>451</v>
       </c>
@@ -16770,7 +16803,7 @@
       <c r="M1" s="742"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="676"/>
+      <c r="B2" s="700"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -16780,21 +16813,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="679" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="680"/>
+      <c r="B3" s="703" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="704"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="681" t="s">
+      <c r="H3" s="705" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="681"/>
+      <c r="I3" s="705"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="718" t="s">
+      <c r="P3" s="729" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="739" t="s">
@@ -16812,14 +16845,14 @@
       <c r="D4" s="18">
         <v>44619</v>
       </c>
-      <c r="E4" s="682" t="s">
+      <c r="E4" s="706" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="683"/>
-      <c r="H4" s="684" t="s">
+      <c r="F4" s="707"/>
+      <c r="H4" s="708" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="685"/>
+      <c r="I4" s="709"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -16829,15 +16862,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="719"/>
+      <c r="P4" s="730"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="740"/>
-      <c r="W4" s="728" t="s">
+      <c r="W4" s="712" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="728"/>
+      <c r="X4" s="712"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -16888,8 +16921,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="728"/>
-      <c r="X5" s="728"/>
+      <c r="W5" s="712"/>
+      <c r="X5" s="712"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -17652,7 +17685,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="732">
+      <c r="W19" s="716">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -17704,7 +17737,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="733"/>
+      <c r="W20" s="717"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -17753,8 +17786,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="734"/>
-      <c r="X21" s="734"/>
+      <c r="W21" s="718"/>
+      <c r="X21" s="718"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -17854,8 +17887,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="735"/>
-      <c r="X23" s="735"/>
+      <c r="W23" s="719"/>
+      <c r="X23" s="719"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -17910,8 +17943,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="735"/>
-      <c r="X24" s="735"/>
+      <c r="W24" s="719"/>
+      <c r="X24" s="719"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -17959,8 +17992,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="736"/>
-      <c r="X25" s="736"/>
+      <c r="W25" s="720"/>
+      <c r="X25" s="720"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -18009,8 +18042,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="736"/>
-      <c r="X26" s="736"/>
+      <c r="W26" s="720"/>
+      <c r="X26" s="720"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -18058,9 +18091,9 @@
       <c r="R27" s="388">
         <v>170</v>
       </c>
-      <c r="W27" s="729"/>
-      <c r="X27" s="730"/>
-      <c r="Y27" s="731"/>
+      <c r="W27" s="713"/>
+      <c r="X27" s="714"/>
+      <c r="Y27" s="715"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -18108,9 +18141,9 @@
       <c r="R28" s="388">
         <v>37374.36</v>
       </c>
-      <c r="W28" s="730"/>
-      <c r="X28" s="730"/>
-      <c r="Y28" s="731"/>
+      <c r="W28" s="714"/>
+      <c r="X28" s="714"/>
+      <c r="Y28" s="715"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -18442,11 +18475,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="720">
+      <c r="M36" s="731">
         <f>SUM(M5:M35)</f>
         <v>2220612.02</v>
       </c>
-      <c r="N36" s="722">
+      <c r="N36" s="733">
         <f>SUM(N5:N35)</f>
         <v>833865</v>
       </c>
@@ -18479,8 +18512,8 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="721"/>
-      <c r="N37" s="723"/>
+      <c r="M37" s="732"/>
+      <c r="N37" s="734"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
@@ -19167,26 +19200,26 @@
       <c r="A68" s="98"/>
       <c r="B68" s="99"/>
       <c r="C68" s="1"/>
-      <c r="H68" s="697" t="s">
+      <c r="H68" s="686" t="s">
         <v>11</v>
       </c>
-      <c r="I68" s="698"/>
+      <c r="I68" s="687"/>
       <c r="J68" s="100"/>
-      <c r="K68" s="699">
+      <c r="K68" s="688">
         <f>I66+L66</f>
         <v>314868.39999999997</v>
       </c>
-      <c r="L68" s="726"/>
+      <c r="L68" s="721"/>
       <c r="M68" s="272"/>
       <c r="N68" s="272"/>
       <c r="P68" s="34"/>
       <c r="Q68" s="13"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D69" s="703" t="s">
+      <c r="D69" s="692" t="s">
         <v>12</v>
       </c>
-      <c r="E69" s="703"/>
+      <c r="E69" s="692"/>
       <c r="F69" s="312">
         <f>F66-K68-C66</f>
         <v>1594593.8500000003</v>
@@ -19195,22 +19228,22 @@
       <c r="J69" s="103"/>
     </row>
     <row r="70" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D70" s="727" t="s">
+      <c r="D70" s="722" t="s">
         <v>95</v>
       </c>
-      <c r="E70" s="727"/>
+      <c r="E70" s="722"/>
       <c r="F70" s="111">
         <v>-1360260.32</v>
       </c>
-      <c r="I70" s="704" t="s">
+      <c r="I70" s="693" t="s">
         <v>13</v>
       </c>
-      <c r="J70" s="705"/>
-      <c r="K70" s="706">
+      <c r="J70" s="694"/>
+      <c r="K70" s="695">
         <f>F72+F73+F74</f>
         <v>1938640.11</v>
       </c>
-      <c r="L70" s="706"/>
+      <c r="L70" s="695"/>
       <c r="M70" s="404"/>
       <c r="N70" s="404"/>
       <c r="O70" s="404"/>
@@ -19251,11 +19284,11 @@
         <v>15</v>
       </c>
       <c r="J72" s="109"/>
-      <c r="K72" s="708">
+      <c r="K72" s="697">
         <f>-C4</f>
         <v>-1266568.45</v>
       </c>
-      <c r="L72" s="709"/>
+      <c r="L72" s="698"/>
     </row>
     <row r="73" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D73" s="110" t="s">
@@ -19272,22 +19305,22 @@
       <c r="C74" s="112">
         <v>44647</v>
       </c>
-      <c r="D74" s="686" t="s">
+      <c r="D74" s="675" t="s">
         <v>18</v>
       </c>
-      <c r="E74" s="687"/>
+      <c r="E74" s="676"/>
       <c r="F74" s="113">
         <v>1792817.68</v>
       </c>
-      <c r="I74" s="688" t="s">
+      <c r="I74" s="677" t="s">
         <v>198</v>
       </c>
-      <c r="J74" s="689"/>
-      <c r="K74" s="690">
+      <c r="J74" s="678"/>
+      <c r="K74" s="679">
         <f>K70+K72</f>
         <v>672071.66000000015</v>
       </c>
-      <c r="L74" s="690"/>
+      <c r="L74" s="679"/>
     </row>
     <row r="75" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C75" s="114"/>
@@ -19430,10 +19463,25 @@
       <c r="F96" s="129"/>
     </row>
   </sheetData>
-  <sortState ref="B34:D42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B34:D42">
     <sortCondition ref="B34:B42"/>
   </sortState>
   <mergeCells count="30">
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="M39:N39"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -19449,21 +19497,6 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
   </mergeCells>
   <pageMargins left="0.27559055118110237" right="0.15748031496062992" top="0.39370078740157483" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -19473,7 +19506,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
@@ -22013,7 +22046,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -22049,7 +22082,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="675"/>
+      <c r="B1" s="699"/>
       <c r="C1" s="741" t="s">
         <v>620</v>
       </c>
@@ -22065,7 +22098,7 @@
       <c r="M1" s="742"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="676"/>
+      <c r="B2" s="700"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -22075,21 +22108,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="679" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="680"/>
+      <c r="B3" s="703" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="704"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="681" t="s">
+      <c r="H3" s="705" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="681"/>
+      <c r="I3" s="705"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="718" t="s">
+      <c r="P3" s="729" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="739" t="s">
@@ -22107,14 +22140,14 @@
       <c r="D4" s="18">
         <v>44647</v>
       </c>
-      <c r="E4" s="682" t="s">
+      <c r="E4" s="706" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="683"/>
-      <c r="H4" s="684" t="s">
+      <c r="F4" s="707"/>
+      <c r="H4" s="708" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="685"/>
+      <c r="I4" s="709"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -22124,15 +22157,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="719"/>
+      <c r="P4" s="730"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="740"/>
-      <c r="W4" s="728" t="s">
+      <c r="W4" s="712" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="728"/>
+      <c r="X4" s="712"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -22183,8 +22216,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="728"/>
-      <c r="X5" s="728"/>
+      <c r="W5" s="712"/>
+      <c r="X5" s="712"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -22943,7 +22976,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="732">
+      <c r="W19" s="716">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -22995,7 +23028,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="733"/>
+      <c r="W20" s="717"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -23044,8 +23077,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="734"/>
-      <c r="X21" s="734"/>
+      <c r="W21" s="718"/>
+      <c r="X21" s="718"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -23142,8 +23175,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="735"/>
-      <c r="X23" s="735"/>
+      <c r="W23" s="719"/>
+      <c r="X23" s="719"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -23198,8 +23231,8 @@
         <v>642</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="735"/>
-      <c r="X24" s="735"/>
+      <c r="W24" s="719"/>
+      <c r="X24" s="719"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -23245,8 +23278,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="736"/>
-      <c r="X25" s="736"/>
+      <c r="W25" s="720"/>
+      <c r="X25" s="720"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -23297,8 +23330,8 @@
       <c r="R26" s="388">
         <v>73524.61</v>
       </c>
-      <c r="W26" s="736"/>
-      <c r="X26" s="736"/>
+      <c r="W26" s="720"/>
+      <c r="X26" s="720"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -23349,9 +23382,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="729"/>
-      <c r="X27" s="730"/>
-      <c r="Y27" s="731"/>
+      <c r="W27" s="713"/>
+      <c r="X27" s="714"/>
+      <c r="Y27" s="715"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -23401,9 +23434,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="730"/>
-      <c r="X28" s="730"/>
-      <c r="Y28" s="731"/>
+      <c r="W28" s="714"/>
+      <c r="X28" s="714"/>
+      <c r="Y28" s="715"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -24007,11 +24040,11 @@
       <c r="L41" s="627">
         <v>15798.5</v>
       </c>
-      <c r="M41" s="720">
+      <c r="M41" s="731">
         <f>SUM(M5:M40)</f>
         <v>2479367.6100000003</v>
       </c>
-      <c r="N41" s="720">
+      <c r="N41" s="731">
         <f>SUM(N5:N40)</f>
         <v>1195667</v>
       </c>
@@ -24049,8 +24082,8 @@
       <c r="L42" s="630">
         <v>15298.5</v>
       </c>
-      <c r="M42" s="721"/>
-      <c r="N42" s="721"/>
+      <c r="M42" s="732"/>
+      <c r="N42" s="732"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="780"/>
     </row>
@@ -24737,26 +24770,26 @@
       <c r="A70" s="98"/>
       <c r="B70" s="99"/>
       <c r="C70" s="1"/>
-      <c r="H70" s="697" t="s">
+      <c r="H70" s="686" t="s">
         <v>11</v>
       </c>
-      <c r="I70" s="698"/>
+      <c r="I70" s="687"/>
       <c r="J70" s="100"/>
-      <c r="K70" s="699">
+      <c r="K70" s="688">
         <f>I68+L68</f>
         <v>428155.54000000004</v>
       </c>
-      <c r="L70" s="726"/>
+      <c r="L70" s="721"/>
       <c r="M70" s="272"/>
       <c r="N70" s="272"/>
       <c r="P70" s="34"/>
       <c r="Q70" s="13"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D71" s="703" t="s">
+      <c r="D71" s="692" t="s">
         <v>12</v>
       </c>
-      <c r="E71" s="703"/>
+      <c r="E71" s="692"/>
       <c r="F71" s="312">
         <f>F68-K70-C68</f>
         <v>1631087.67</v>
@@ -24766,22 +24799,22 @@
       <c r="P71" s="34"/>
     </row>
     <row r="72" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D72" s="727" t="s">
+      <c r="D72" s="722" t="s">
         <v>95</v>
       </c>
-      <c r="E72" s="727"/>
+      <c r="E72" s="722"/>
       <c r="F72" s="111">
         <v>-1884975.46</v>
       </c>
-      <c r="I72" s="704" t="s">
+      <c r="I72" s="693" t="s">
         <v>13</v>
       </c>
-      <c r="J72" s="705"/>
-      <c r="K72" s="706">
+      <c r="J72" s="694"/>
+      <c r="K72" s="695">
         <f>F74+F75+F76</f>
         <v>1777829.89</v>
       </c>
-      <c r="L72" s="706"/>
+      <c r="L72" s="695"/>
       <c r="M72" s="404"/>
       <c r="N72" s="404"/>
       <c r="O72" s="404"/>
@@ -24822,11 +24855,11 @@
         <v>15</v>
       </c>
       <c r="J74" s="109"/>
-      <c r="K74" s="708">
+      <c r="K74" s="697">
         <f>-C4</f>
         <v>-1792817.68</v>
       </c>
-      <c r="L74" s="709"/>
+      <c r="L74" s="698"/>
       <c r="P74" s="34"/>
     </row>
     <row r="75" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -24845,22 +24878,22 @@
       <c r="C76" s="112">
         <v>44682</v>
       </c>
-      <c r="D76" s="686" t="s">
+      <c r="D76" s="675" t="s">
         <v>18</v>
       </c>
-      <c r="E76" s="687"/>
+      <c r="E76" s="676"/>
       <c r="F76" s="113">
         <v>2112071.92</v>
       </c>
-      <c r="I76" s="688" t="s">
+      <c r="I76" s="677" t="s">
         <v>854</v>
       </c>
-      <c r="J76" s="689"/>
-      <c r="K76" s="690">
+      <c r="J76" s="678"/>
+      <c r="K76" s="679">
         <f>K72+K74</f>
         <v>-14987.790000000037</v>
       </c>
-      <c r="L76" s="690"/>
+      <c r="L76" s="679"/>
       <c r="P76" s="34"/>
     </row>
     <row r="77" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
@@ -25016,10 +25049,25 @@
       <c r="F98" s="129"/>
     </row>
   </sheetData>
-  <sortState ref="J47:L67">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J47:L67">
     <sortCondition ref="J47:J67"/>
   </sortState>
   <mergeCells count="30">
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="M45:N45"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -25035,21 +25083,6 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="K72:L72"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -25059,7 +25092,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -28071,7 +28104,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -28306,7 +28339,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFCC99FF"/>
   </sheetPr>
@@ -28346,7 +28379,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="675"/>
+      <c r="B1" s="699"/>
       <c r="C1" s="741" t="s">
         <v>754</v>
       </c>
@@ -28362,7 +28395,7 @@
       <c r="M1" s="742"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="676"/>
+      <c r="B2" s="700"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -28372,21 +28405,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="679" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="680"/>
+      <c r="B3" s="703" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="704"/>
       <c r="D3" s="10"/>
       <c r="E3" s="556"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="681" t="s">
+      <c r="H3" s="705" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="681"/>
+      <c r="I3" s="705"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="718" t="s">
+      <c r="P3" s="729" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="739" t="s">
@@ -28408,14 +28441,14 @@
       <c r="D4" s="18">
         <v>44682</v>
       </c>
-      <c r="E4" s="682" t="s">
+      <c r="E4" s="706" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="683"/>
-      <c r="H4" s="684" t="s">
+      <c r="F4" s="707"/>
+      <c r="H4" s="708" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="685"/>
+      <c r="I4" s="709"/>
       <c r="J4" s="559"/>
       <c r="K4" s="565"/>
       <c r="L4" s="566"/>
@@ -28425,15 +28458,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="719"/>
+      <c r="P4" s="730"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="740"/>
       <c r="U4" s="34"/>
       <c r="V4" s="128"/>
-      <c r="W4" s="801"/>
-      <c r="X4" s="801"/>
+      <c r="W4" s="804"/>
+      <c r="X4" s="804"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -28487,8 +28520,8 @@
       <c r="S5" s="324"/>
       <c r="U5" s="34"/>
       <c r="V5" s="128"/>
-      <c r="W5" s="801"/>
-      <c r="X5" s="801"/>
+      <c r="W5" s="804"/>
+      <c r="X5" s="804"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -29254,7 +29287,7 @@
       <c r="S19" s="147"/>
       <c r="U19" s="34"/>
       <c r="V19" s="128"/>
-      <c r="W19" s="802"/>
+      <c r="W19" s="805"/>
       <c r="X19" s="544"/>
       <c r="Y19" s="233"/>
     </row>
@@ -29308,7 +29341,7 @@
       <c r="S20" s="147"/>
       <c r="U20" s="34"/>
       <c r="V20" s="128"/>
-      <c r="W20" s="802"/>
+      <c r="W20" s="805"/>
       <c r="X20" s="34"/>
       <c r="Y20" s="233"/>
     </row>
@@ -29363,8 +29396,8 @@
       <c r="S21" s="147"/>
       <c r="U21" s="34"/>
       <c r="V21" s="128"/>
-      <c r="W21" s="734"/>
-      <c r="X21" s="734"/>
+      <c r="W21" s="718"/>
+      <c r="X21" s="718"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -29475,8 +29508,8 @@
       <c r="S23" s="147"/>
       <c r="U23" s="34"/>
       <c r="V23" s="128"/>
-      <c r="W23" s="735"/>
-      <c r="X23" s="735"/>
+      <c r="W23" s="719"/>
+      <c r="X23" s="719"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -29537,8 +29570,8 @@
       <c r="S24" s="147"/>
       <c r="U24" s="34"/>
       <c r="V24" s="128"/>
-      <c r="W24" s="735"/>
-      <c r="X24" s="735"/>
+      <c r="W24" s="719"/>
+      <c r="X24" s="719"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -29591,8 +29624,8 @@
       </c>
       <c r="U25" s="34"/>
       <c r="V25" s="128"/>
-      <c r="W25" s="736"/>
-      <c r="X25" s="736"/>
+      <c r="W25" s="720"/>
+      <c r="X25" s="720"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -29647,8 +29680,8 @@
       <c r="T26" s="128"/>
       <c r="U26" s="34"/>
       <c r="V26" s="128"/>
-      <c r="W26" s="736"/>
-      <c r="X26" s="736"/>
+      <c r="W26" s="720"/>
+      <c r="X26" s="720"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -29703,9 +29736,9 @@
       <c r="T27" s="128"/>
       <c r="U27" s="34"/>
       <c r="V27" s="128"/>
-      <c r="W27" s="729"/>
-      <c r="X27" s="730"/>
-      <c r="Y27" s="731"/>
+      <c r="W27" s="713"/>
+      <c r="X27" s="714"/>
+      <c r="Y27" s="715"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -29759,9 +29792,9 @@
       <c r="T28" s="128"/>
       <c r="U28" s="34"/>
       <c r="V28" s="128"/>
-      <c r="W28" s="730"/>
-      <c r="X28" s="730"/>
-      <c r="Y28" s="731"/>
+      <c r="W28" s="714"/>
+      <c r="X28" s="714"/>
+      <c r="Y28" s="715"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -30352,11 +30385,11 @@
       <c r="J41" s="56"/>
       <c r="K41" s="38"/>
       <c r="L41" s="39"/>
-      <c r="M41" s="720">
+      <c r="M41" s="731">
         <f>SUM(M5:M40)</f>
         <v>1509924.1</v>
       </c>
-      <c r="N41" s="720">
+      <c r="N41" s="731">
         <f>SUM(N5:N40)</f>
         <v>1012291</v>
       </c>
@@ -30388,8 +30421,8 @@
       <c r="L42" s="641">
         <v>3095.88</v>
       </c>
-      <c r="M42" s="721"/>
-      <c r="N42" s="721"/>
+      <c r="M42" s="732"/>
+      <c r="N42" s="732"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="780"/>
     </row>
@@ -30880,26 +30913,26 @@
       <c r="A63" s="98"/>
       <c r="B63" s="99"/>
       <c r="C63" s="1"/>
-      <c r="H63" s="697" t="s">
+      <c r="H63" s="686" t="s">
         <v>11</v>
       </c>
-      <c r="I63" s="698"/>
+      <c r="I63" s="687"/>
       <c r="J63" s="562"/>
-      <c r="K63" s="804">
+      <c r="K63" s="801">
         <f>I61+L61</f>
         <v>340912.75</v>
       </c>
-      <c r="L63" s="805"/>
+      <c r="L63" s="802"/>
       <c r="M63" s="272"/>
       <c r="N63" s="272"/>
       <c r="P63" s="34"/>
       <c r="Q63" s="13"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D64" s="703" t="s">
+      <c r="D64" s="692" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="703"/>
+      <c r="E64" s="692"/>
       <c r="F64" s="312">
         <f>F61-K63-C61</f>
         <v>1458827.53</v>
@@ -30908,22 +30941,22 @@
       <c r="J64" s="563"/>
     </row>
     <row r="65" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D65" s="727" t="s">
+      <c r="D65" s="722" t="s">
         <v>95</v>
       </c>
-      <c r="E65" s="727"/>
+      <c r="E65" s="722"/>
       <c r="F65" s="111">
         <v>-1572197.3</v>
       </c>
-      <c r="I65" s="704" t="s">
+      <c r="I65" s="693" t="s">
         <v>13</v>
       </c>
-      <c r="J65" s="705"/>
-      <c r="K65" s="706">
+      <c r="J65" s="694"/>
+      <c r="K65" s="695">
         <f>F67+F68+F69</f>
         <v>2392765.5300000003</v>
       </c>
-      <c r="L65" s="706"/>
+      <c r="L65" s="695"/>
       <c r="M65" s="404"/>
       <c r="N65" s="404"/>
       <c r="O65" s="582"/>
@@ -30968,7 +31001,7 @@
         <f>-C4</f>
         <v>-2112071.92</v>
       </c>
-      <c r="L67" s="706"/>
+      <c r="L67" s="695"/>
     </row>
     <row r="68" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="110" t="s">
@@ -30985,22 +31018,22 @@
       <c r="C69" s="112">
         <v>44710</v>
       </c>
-      <c r="D69" s="686" t="s">
+      <c r="D69" s="675" t="s">
         <v>18</v>
       </c>
-      <c r="E69" s="687"/>
+      <c r="E69" s="676"/>
       <c r="F69" s="113">
         <v>2546982.16</v>
       </c>
-      <c r="I69" s="688" t="s">
+      <c r="I69" s="677" t="s">
         <v>198</v>
       </c>
-      <c r="J69" s="689"/>
-      <c r="K69" s="690">
+      <c r="J69" s="678"/>
+      <c r="K69" s="679">
         <f>K65+K67</f>
         <v>280693.61000000034</v>
       </c>
-      <c r="L69" s="690"/>
+      <c r="L69" s="679"/>
     </row>
     <row r="70" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C70" s="114"/>
@@ -31143,25 +31176,10 @@
       <c r="F91" s="129"/>
     </row>
   </sheetData>
-  <sortState ref="J42:L56">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J42:L56">
     <sortCondition ref="J42:J56"/>
   </sortState>
   <mergeCells count="30">
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="K69:L69"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="K63:L63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="K65:L65"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="K67:L67"/>
-    <mergeCell ref="M45:N45"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -31177,6 +31195,21 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="K65:L65"/>
   </mergeCells>
   <pageMargins left="0.28000000000000003" right="0.19" top="0.33" bottom="0.33" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -31186,7 +31219,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFCC99FF"/>
   </sheetPr>
@@ -33512,7 +33545,7 @@
       <c r="K106" s="154"/>
     </row>
   </sheetData>
-  <sortState ref="A18:C19">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:C19">
     <sortCondition ref="B18:B19"/>
   </sortState>
   <mergeCells count="5">
@@ -33528,13 +33561,13 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF00FF"/>
   </sheetPr>
   <dimension ref="A1:Z91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
@@ -33565,7 +33598,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="675"/>
+      <c r="B1" s="699"/>
       <c r="C1" s="741" t="s">
         <v>886</v>
       </c>
@@ -33581,7 +33614,7 @@
       <c r="M1" s="742"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="676"/>
+      <c r="B2" s="700"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -33591,21 +33624,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="679" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="680"/>
+      <c r="B3" s="703" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="704"/>
       <c r="D3" s="10"/>
       <c r="E3" s="556"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="681" t="s">
+      <c r="H3" s="705" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="681"/>
+      <c r="I3" s="705"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="718" t="s">
+      <c r="P3" s="729" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="739" t="s">
@@ -33627,14 +33660,14 @@
       <c r="D4" s="18">
         <v>44710</v>
       </c>
-      <c r="E4" s="682" t="s">
+      <c r="E4" s="706" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="683"/>
-      <c r="H4" s="684" t="s">
+      <c r="F4" s="707"/>
+      <c r="H4" s="708" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="685"/>
+      <c r="I4" s="709"/>
       <c r="J4" s="559"/>
       <c r="K4" s="565"/>
       <c r="L4" s="566"/>
@@ -33644,15 +33677,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="719"/>
+      <c r="P4" s="730"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="740"/>
       <c r="U4" s="34"/>
       <c r="V4" s="128"/>
-      <c r="W4" s="801"/>
-      <c r="X4" s="801"/>
+      <c r="W4" s="804"/>
+      <c r="X4" s="804"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -33707,8 +33740,8 @@
       <c r="S5" s="324"/>
       <c r="U5" s="34"/>
       <c r="V5" s="128"/>
-      <c r="W5" s="801"/>
-      <c r="X5" s="801"/>
+      <c r="W5" s="804"/>
+      <c r="X5" s="804"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -34484,7 +34517,7 @@
       <c r="S19" s="147"/>
       <c r="U19" s="34"/>
       <c r="V19" s="128"/>
-      <c r="W19" s="802"/>
+      <c r="W19" s="805"/>
       <c r="X19" s="544"/>
       <c r="Y19" s="233"/>
     </row>
@@ -34538,7 +34571,7 @@
       <c r="S20" s="147"/>
       <c r="U20" s="34"/>
       <c r="V20" s="128"/>
-      <c r="W20" s="802"/>
+      <c r="W20" s="805"/>
       <c r="X20" s="34"/>
       <c r="Y20" s="233"/>
     </row>
@@ -34592,8 +34625,8 @@
       <c r="S21" s="147"/>
       <c r="U21" s="34"/>
       <c r="V21" s="128"/>
-      <c r="W21" s="734"/>
-      <c r="X21" s="734"/>
+      <c r="W21" s="718"/>
+      <c r="X21" s="718"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -34702,8 +34735,8 @@
       <c r="S23" s="147"/>
       <c r="U23" s="34"/>
       <c r="V23" s="128"/>
-      <c r="W23" s="735"/>
-      <c r="X23" s="735"/>
+      <c r="W23" s="719"/>
+      <c r="X23" s="719"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -34763,8 +34796,8 @@
       <c r="S24" s="147"/>
       <c r="U24" s="34"/>
       <c r="V24" s="128"/>
-      <c r="W24" s="735"/>
-      <c r="X24" s="735"/>
+      <c r="W24" s="719"/>
+      <c r="X24" s="719"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -34817,8 +34850,8 @@
       </c>
       <c r="U25" s="34"/>
       <c r="V25" s="128"/>
-      <c r="W25" s="736"/>
-      <c r="X25" s="736"/>
+      <c r="W25" s="720"/>
+      <c r="X25" s="720"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -34873,8 +34906,8 @@
       <c r="T26" s="128"/>
       <c r="U26" s="34"/>
       <c r="V26" s="128"/>
-      <c r="W26" s="736"/>
-      <c r="X26" s="736"/>
+      <c r="W26" s="720"/>
+      <c r="X26" s="720"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -34929,9 +34962,9 @@
       <c r="T27" s="128"/>
       <c r="U27" s="34"/>
       <c r="V27" s="128"/>
-      <c r="W27" s="729"/>
-      <c r="X27" s="730"/>
-      <c r="Y27" s="731"/>
+      <c r="W27" s="713"/>
+      <c r="X27" s="714"/>
+      <c r="Y27" s="715"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -34986,9 +35019,9 @@
       <c r="T28" s="128"/>
       <c r="U28" s="34"/>
       <c r="V28" s="128"/>
-      <c r="W28" s="730"/>
-      <c r="X28" s="730"/>
-      <c r="Y28" s="731"/>
+      <c r="W28" s="714"/>
+      <c r="X28" s="714"/>
+      <c r="Y28" s="715"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -35645,11 +35678,11 @@
       <c r="L41" s="39">
         <v>18992.37</v>
       </c>
-      <c r="M41" s="720">
+      <c r="M41" s="731">
         <f>SUM(M5:M40)</f>
         <v>1737024</v>
       </c>
-      <c r="N41" s="720">
+      <c r="N41" s="731">
         <f>SUM(N5:N40)</f>
         <v>1314313</v>
       </c>
@@ -35681,8 +35714,8 @@
       <c r="L42" s="52">
         <v>17035.3</v>
       </c>
-      <c r="M42" s="721"/>
-      <c r="N42" s="721"/>
+      <c r="M42" s="732"/>
+      <c r="N42" s="732"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="780"/>
     </row>
@@ -36100,26 +36133,26 @@
       <c r="A63" s="98"/>
       <c r="B63" s="99"/>
       <c r="C63" s="1"/>
-      <c r="H63" s="697" t="s">
+      <c r="H63" s="686" t="s">
         <v>11</v>
       </c>
-      <c r="I63" s="698"/>
+      <c r="I63" s="687"/>
       <c r="J63" s="562"/>
-      <c r="K63" s="804">
+      <c r="K63" s="801">
         <f>I61+L61</f>
         <v>299758.48</v>
       </c>
-      <c r="L63" s="805"/>
+      <c r="L63" s="802"/>
       <c r="M63" s="272"/>
       <c r="N63" s="272"/>
       <c r="P63" s="34"/>
       <c r="Q63" s="13"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D64" s="703" t="s">
+      <c r="D64" s="692" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="703"/>
+      <c r="E64" s="692"/>
       <c r="F64" s="312">
         <f>F61-K63-C61</f>
         <v>2910425.02</v>
@@ -36128,22 +36161,22 @@
       <c r="J64" s="563"/>
     </row>
     <row r="65" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D65" s="727" t="s">
+      <c r="D65" s="722" t="s">
         <v>95</v>
       </c>
-      <c r="E65" s="727"/>
+      <c r="E65" s="722"/>
       <c r="F65" s="111">
         <v>-2122394.9</v>
       </c>
-      <c r="I65" s="704" t="s">
+      <c r="I65" s="693" t="s">
         <v>13</v>
       </c>
-      <c r="J65" s="705"/>
-      <c r="K65" s="706">
+      <c r="J65" s="694"/>
+      <c r="K65" s="695">
         <f>F67+F68+F69</f>
         <v>3684164.66</v>
       </c>
-      <c r="L65" s="706"/>
+      <c r="L65" s="695"/>
       <c r="M65" s="404"/>
       <c r="N65" s="404"/>
       <c r="O65" s="659"/>
@@ -36188,7 +36221,7 @@
         <f>-C4</f>
         <v>-2546982.16</v>
       </c>
-      <c r="L67" s="706"/>
+      <c r="L67" s="695"/>
     </row>
     <row r="68" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="110" t="s">
@@ -36205,22 +36238,22 @@
       <c r="C69" s="112">
         <v>44745</v>
       </c>
-      <c r="D69" s="686" t="s">
+      <c r="D69" s="675" t="s">
         <v>18</v>
       </c>
-      <c r="E69" s="687"/>
+      <c r="E69" s="676"/>
       <c r="F69" s="113">
         <v>2355426.54</v>
       </c>
-      <c r="I69" s="688" t="s">
+      <c r="I69" s="677" t="s">
         <v>198</v>
       </c>
-      <c r="J69" s="689"/>
-      <c r="K69" s="690">
+      <c r="J69" s="678"/>
+      <c r="K69" s="679">
         <f>K65+K67</f>
         <v>1137182.5</v>
       </c>
-      <c r="L69" s="690"/>
+      <c r="L69" s="679"/>
     </row>
     <row r="70" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C70" s="114"/>
@@ -36364,6 +36397,26 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="K67:L67"/>
     <mergeCell ref="D69:E69"/>
     <mergeCell ref="I69:J69"/>
     <mergeCell ref="K69:L69"/>
@@ -36374,26 +36427,6 @@
     <mergeCell ref="D65:E65"/>
     <mergeCell ref="I65:J65"/>
     <mergeCell ref="K65:L65"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="K67:L67"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -36403,7 +36436,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF00FF"/>
   </sheetPr>
@@ -38685,7 +38718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF800000"/>
   </sheetPr>
@@ -41609,7 +41642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -41621,7 +41654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -41633,7 +41666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -41668,23 +41701,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="675"/>
-      <c r="C1" s="677" t="s">
+      <c r="B1" s="699"/>
+      <c r="C1" s="701" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="678"/>
-      <c r="E1" s="678"/>
-      <c r="F1" s="678"/>
-      <c r="G1" s="678"/>
-      <c r="H1" s="678"/>
-      <c r="I1" s="678"/>
-      <c r="J1" s="678"/>
-      <c r="K1" s="678"/>
-      <c r="L1" s="678"/>
-      <c r="M1" s="678"/>
+      <c r="D1" s="702"/>
+      <c r="E1" s="702"/>
+      <c r="F1" s="702"/>
+      <c r="G1" s="702"/>
+      <c r="H1" s="702"/>
+      <c r="I1" s="702"/>
+      <c r="J1" s="702"/>
+      <c r="K1" s="702"/>
+      <c r="L1" s="702"/>
+      <c r="M1" s="702"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="676"/>
+      <c r="B2" s="700"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -41694,21 +41727,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="679" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="680"/>
+      <c r="B3" s="703" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="704"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="681" t="s">
+      <c r="H3" s="705" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="681"/>
+      <c r="I3" s="705"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="718" t="s">
+      <c r="P3" s="729" t="s">
         <v>6</v>
       </c>
     </row>
@@ -41723,14 +41756,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="682" t="s">
+      <c r="E4" s="706" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="683"/>
-      <c r="H4" s="684" t="s">
+      <c r="F4" s="707"/>
+      <c r="H4" s="708" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="685"/>
+      <c r="I4" s="709"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -41740,14 +41773,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="719"/>
+      <c r="P4" s="730"/>
       <c r="Q4" s="286" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="728" t="s">
+      <c r="W4" s="712" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="728"/>
+      <c r="X4" s="712"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -41798,8 +41831,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="728"/>
-      <c r="X5" s="728"/>
+      <c r="W5" s="712"/>
+      <c r="X5" s="712"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -42570,7 +42603,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="732">
+      <c r="W19" s="716">
         <f>SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -42622,7 +42655,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="733"/>
+      <c r="W20" s="717"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -42671,8 +42704,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="734"/>
-      <c r="X21" s="734"/>
+      <c r="W21" s="718"/>
+      <c r="X21" s="718"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -42773,8 +42806,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="735"/>
-      <c r="X23" s="735"/>
+      <c r="W23" s="719"/>
+      <c r="X23" s="719"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -42828,8 +42861,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="735"/>
-      <c r="X24" s="735"/>
+      <c r="W24" s="719"/>
+      <c r="X24" s="719"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -42875,8 +42908,8 @@
       <c r="R25" s="285">
         <v>28952</v>
       </c>
-      <c r="W25" s="736"/>
-      <c r="X25" s="736"/>
+      <c r="W25" s="720"/>
+      <c r="X25" s="720"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -42927,8 +42960,8 @@
       <c r="R26" s="285">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="736"/>
-      <c r="X26" s="736"/>
+      <c r="W26" s="720"/>
+      <c r="X26" s="720"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -42976,9 +43009,9 @@
       <c r="R27" s="285">
         <v>14637</v>
       </c>
-      <c r="W27" s="729"/>
-      <c r="X27" s="730"/>
-      <c r="Y27" s="731"/>
+      <c r="W27" s="713"/>
+      <c r="X27" s="714"/>
+      <c r="Y27" s="715"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -43028,9 +43061,9 @@
       <c r="R28" s="285">
         <v>0</v>
       </c>
-      <c r="W28" s="730"/>
-      <c r="X28" s="730"/>
-      <c r="Y28" s="731"/>
+      <c r="W28" s="714"/>
+      <c r="X28" s="714"/>
+      <c r="Y28" s="715"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -43365,11 +43398,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="720">
+      <c r="M36" s="731">
         <f>SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="722">
+      <c r="N36" s="733">
         <f>SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -43377,7 +43410,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="724">
+      <c r="Q36" s="735">
         <f>SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -43412,13 +43445,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="721"/>
-      <c r="N37" s="723"/>
+      <c r="M37" s="732"/>
+      <c r="N37" s="734"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="725"/>
+      <c r="Q37" s="736"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -43708,26 +43741,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="697" t="s">
+      <c r="H52" s="686" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="698"/>
+      <c r="I52" s="687"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="699">
+      <c r="K52" s="688">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="726"/>
+      <c r="L52" s="721"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="703" t="s">
+      <c r="D53" s="692" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="703"/>
+      <c r="E53" s="692"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -43736,29 +43769,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="727" t="s">
+      <c r="D54" s="722" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="727"/>
+      <c r="E54" s="722"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="704" t="s">
+      <c r="I54" s="693" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="705"/>
-      <c r="K54" s="706">
+      <c r="J54" s="694"/>
+      <c r="K54" s="695">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="706"/>
-      <c r="M54" s="712" t="s">
+      <c r="L54" s="695"/>
+      <c r="M54" s="723" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="713"/>
-      <c r="O54" s="713"/>
-      <c r="P54" s="713"/>
-      <c r="Q54" s="714"/>
+      <c r="N54" s="724"/>
+      <c r="O54" s="724"/>
+      <c r="P54" s="724"/>
+      <c r="Q54" s="725"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -43772,11 +43805,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="715"/>
-      <c r="N55" s="716"/>
-      <c r="O55" s="716"/>
-      <c r="P55" s="716"/>
-      <c r="Q55" s="717"/>
+      <c r="M55" s="726"/>
+      <c r="N55" s="727"/>
+      <c r="O55" s="727"/>
+      <c r="P55" s="727"/>
+      <c r="Q55" s="728"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -43794,11 +43827,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="708">
+      <c r="K56" s="697">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="709"/>
+      <c r="L56" s="698"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -43815,22 +43848,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="686" t="s">
+      <c r="D58" s="675" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="687"/>
+      <c r="E58" s="676"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="688" t="s">
+      <c r="I58" s="677" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="689"/>
-      <c r="K58" s="690">
+      <c r="J58" s="678"/>
+      <c r="K58" s="679">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="690"/>
+      <c r="L58" s="679"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -43974,14 +44007,17 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -43992,17 +44028,14 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.27559055118110237" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="68" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -44012,7 +44045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -46709,7 +46742,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF6600FF"/>
   </sheetPr>
@@ -46745,23 +46778,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="675"/>
-      <c r="C1" s="677" t="s">
+      <c r="B1" s="699"/>
+      <c r="C1" s="701" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="678"/>
-      <c r="E1" s="678"/>
-      <c r="F1" s="678"/>
-      <c r="G1" s="678"/>
-      <c r="H1" s="678"/>
-      <c r="I1" s="678"/>
-      <c r="J1" s="678"/>
-      <c r="K1" s="678"/>
-      <c r="L1" s="678"/>
-      <c r="M1" s="678"/>
+      <c r="D1" s="702"/>
+      <c r="E1" s="702"/>
+      <c r="F1" s="702"/>
+      <c r="G1" s="702"/>
+      <c r="H1" s="702"/>
+      <c r="I1" s="702"/>
+      <c r="J1" s="702"/>
+      <c r="K1" s="702"/>
+      <c r="L1" s="702"/>
+      <c r="M1" s="702"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="676"/>
+      <c r="B2" s="700"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -46771,21 +46804,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="679" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="680"/>
+      <c r="B3" s="703" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="704"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="681" t="s">
+      <c r="H3" s="705" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="681"/>
+      <c r="I3" s="705"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="718" t="s">
+      <c r="P3" s="729" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="739" t="s">
@@ -46803,14 +46836,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="682" t="s">
+      <c r="E4" s="706" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="683"/>
-      <c r="H4" s="684" t="s">
+      <c r="F4" s="707"/>
+      <c r="H4" s="708" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="685"/>
+      <c r="I4" s="709"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -46820,15 +46853,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="719"/>
+      <c r="P4" s="730"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="740"/>
-      <c r="W4" s="728" t="s">
+      <c r="W4" s="712" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="728"/>
+      <c r="X4" s="712"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -46889,8 +46922,8 @@
       <c r="S5" s="324" t="s">
         <v>213</v>
       </c>
-      <c r="W5" s="728"/>
-      <c r="X5" s="728"/>
+      <c r="W5" s="712"/>
+      <c r="X5" s="712"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -47647,7 +47680,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="732">
+      <c r="W19" s="716">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -47699,7 +47732,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="733"/>
+      <c r="W20" s="717"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -47748,8 +47781,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="734"/>
-      <c r="X21" s="734"/>
+      <c r="W21" s="718"/>
+      <c r="X21" s="718"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -47850,8 +47883,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="735"/>
-      <c r="X23" s="735"/>
+      <c r="W23" s="719"/>
+      <c r="X23" s="719"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -47902,8 +47935,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="735"/>
-      <c r="X24" s="735"/>
+      <c r="W24" s="719"/>
+      <c r="X24" s="719"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -47949,8 +47982,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="736"/>
-      <c r="X25" s="736"/>
+      <c r="W25" s="720"/>
+      <c r="X25" s="720"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -47998,8 +48031,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="736"/>
-      <c r="X26" s="736"/>
+      <c r="W26" s="720"/>
+      <c r="X26" s="720"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -48059,9 +48092,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="729"/>
-      <c r="X27" s="730"/>
-      <c r="Y27" s="731"/>
+      <c r="W27" s="713"/>
+      <c r="X27" s="714"/>
+      <c r="Y27" s="715"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -48115,9 +48148,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="730"/>
-      <c r="X28" s="730"/>
-      <c r="Y28" s="731"/>
+      <c r="W28" s="714"/>
+      <c r="X28" s="714"/>
+      <c r="Y28" s="715"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -48433,11 +48466,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="720">
+      <c r="M36" s="731">
         <f>SUM(M5:M35)</f>
         <v>1077791.3</v>
       </c>
-      <c r="N36" s="722">
+      <c r="N36" s="733">
         <f>SUM(N5:N35)</f>
         <v>936398</v>
       </c>
@@ -48445,7 +48478,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="724">
+      <c r="Q36" s="735">
         <f>SUM(Q5:Q35)</f>
         <v>-14262.940000000002</v>
       </c>
@@ -48464,13 +48497,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="721"/>
-      <c r="N37" s="723"/>
+      <c r="M37" s="732"/>
+      <c r="N37" s="734"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="725"/>
+      <c r="Q37" s="736"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -48744,26 +48777,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="697" t="s">
+      <c r="H52" s="686" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="698"/>
+      <c r="I52" s="687"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="699">
+      <c r="K52" s="688">
         <f>I50+L50</f>
         <v>90750.75</v>
       </c>
-      <c r="L52" s="726"/>
+      <c r="L52" s="721"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="703" t="s">
+      <c r="D53" s="692" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="703"/>
+      <c r="E53" s="692"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>1739855.03</v>
@@ -48772,29 +48805,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="727" t="s">
+      <c r="D54" s="722" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="727"/>
+      <c r="E54" s="722"/>
       <c r="F54" s="111">
         <v>-1567070.66</v>
       </c>
-      <c r="I54" s="704" t="s">
+      <c r="I54" s="693" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="705"/>
-      <c r="K54" s="706">
+      <c r="J54" s="694"/>
+      <c r="K54" s="695">
         <f>F56+F57+F58</f>
         <v>703192.8600000001</v>
       </c>
-      <c r="L54" s="706"/>
-      <c r="M54" s="712" t="s">
+      <c r="L54" s="695"/>
+      <c r="M54" s="723" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="713"/>
-      <c r="O54" s="713"/>
-      <c r="P54" s="713"/>
-      <c r="Q54" s="714"/>
+      <c r="N54" s="724"/>
+      <c r="O54" s="724"/>
+      <c r="P54" s="724"/>
+      <c r="Q54" s="725"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -48808,11 +48841,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="715"/>
-      <c r="N55" s="716"/>
-      <c r="O55" s="716"/>
-      <c r="P55" s="716"/>
-      <c r="Q55" s="717"/>
+      <c r="M55" s="726"/>
+      <c r="N55" s="727"/>
+      <c r="O55" s="727"/>
+      <c r="P55" s="727"/>
+      <c r="Q55" s="728"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -48830,11 +48863,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="708">
+      <c r="K56" s="697">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="709"/>
+      <c r="L56" s="698"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -48851,22 +48884,22 @@
       <c r="C58" s="112">
         <v>44563</v>
       </c>
-      <c r="D58" s="686" t="s">
+      <c r="D58" s="675" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="687"/>
+      <c r="E58" s="676"/>
       <c r="F58" s="113">
         <v>754143.23</v>
       </c>
-      <c r="I58" s="688" t="s">
+      <c r="I58" s="677" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="689"/>
-      <c r="K58" s="690">
+      <c r="J58" s="678"/>
+      <c r="K58" s="679">
         <f>K54+K56</f>
         <v>135803.51000000013</v>
       </c>
-      <c r="L58" s="690"/>
+      <c r="L58" s="679"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -49010,20 +49043,13 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="H52:I52"/>
     <mergeCell ref="K52:L52"/>
     <mergeCell ref="W4:X5"/>
@@ -49033,13 +49059,20 @@
     <mergeCell ref="W25:X25"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -49049,7 +49082,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF6600FF"/>
   </sheetPr>
@@ -51698,7 +51731,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -51734,7 +51767,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="675"/>
+      <c r="B1" s="699"/>
       <c r="C1" s="741" t="s">
         <v>316</v>
       </c>
@@ -51750,7 +51783,7 @@
       <c r="M1" s="742"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="676"/>
+      <c r="B2" s="700"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -51760,21 +51793,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="679" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="680"/>
+      <c r="B3" s="703" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="704"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="681" t="s">
+      <c r="H3" s="705" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="681"/>
+      <c r="I3" s="705"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="718" t="s">
+      <c r="P3" s="729" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="739" t="s">
@@ -51792,14 +51825,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="682" t="s">
+      <c r="E4" s="706" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="683"/>
-      <c r="H4" s="684" t="s">
+      <c r="F4" s="707"/>
+      <c r="H4" s="708" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="685"/>
+      <c r="I4" s="709"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -51809,15 +51842,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="719"/>
+      <c r="P4" s="730"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="740"/>
-      <c r="W4" s="728" t="s">
+      <c r="W4" s="712" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="728"/>
+      <c r="X4" s="712"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -51868,8 +51901,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="728"/>
-      <c r="X5" s="728"/>
+      <c r="W5" s="712"/>
+      <c r="X5" s="712"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -52633,7 +52666,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="732">
+      <c r="W19" s="716">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -52686,7 +52719,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="733"/>
+      <c r="W20" s="717"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -52735,8 +52768,8 @@
         <v>377273.87</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="734"/>
-      <c r="X21" s="734"/>
+      <c r="W21" s="718"/>
+      <c r="X21" s="718"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -52836,8 +52869,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="735"/>
-      <c r="X23" s="735"/>
+      <c r="W23" s="719"/>
+      <c r="X23" s="719"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -52892,8 +52925,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="735"/>
-      <c r="X24" s="735"/>
+      <c r="W24" s="719"/>
+      <c r="X24" s="719"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -52938,8 +52971,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="736"/>
-      <c r="X25" s="736"/>
+      <c r="W25" s="720"/>
+      <c r="X25" s="720"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -52987,8 +53020,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="736"/>
-      <c r="X26" s="736"/>
+      <c r="W26" s="720"/>
+      <c r="X26" s="720"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -53042,9 +53075,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="729"/>
-      <c r="X27" s="730"/>
-      <c r="Y27" s="731"/>
+      <c r="W27" s="713"/>
+      <c r="X27" s="714"/>
+      <c r="Y27" s="715"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -53098,9 +53131,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="730"/>
-      <c r="X28" s="730"/>
-      <c r="Y28" s="731"/>
+      <c r="W28" s="714"/>
+      <c r="X28" s="714"/>
+      <c r="Y28" s="715"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -53411,11 +53444,11 @@
       <c r="L36" s="44">
         <v>13275.84</v>
       </c>
-      <c r="M36" s="720">
+      <c r="M36" s="731">
         <f>SUM(M5:M35)</f>
         <v>1818445.73</v>
       </c>
-      <c r="N36" s="722">
+      <c r="N36" s="733">
         <f>SUM(N5:N35)</f>
         <v>739014</v>
       </c>
@@ -53423,7 +53456,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="724">
+      <c r="Q36" s="735">
         <f>SUM(Q5:Q35)</f>
         <v>-7.2800000000133878</v>
       </c>
@@ -53448,13 +53481,13 @@
       <c r="L37" s="61">
         <v>15060.32</v>
       </c>
-      <c r="M37" s="721"/>
-      <c r="N37" s="723"/>
+      <c r="M37" s="732"/>
+      <c r="N37" s="734"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="725"/>
+      <c r="Q37" s="736"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -53747,26 +53780,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="697" t="s">
+      <c r="H52" s="686" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="698"/>
+      <c r="I52" s="687"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="699">
+      <c r="K52" s="688">
         <f>I50+L50</f>
         <v>158798.12</v>
       </c>
-      <c r="L52" s="726"/>
+      <c r="L52" s="721"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="703" t="s">
+      <c r="D53" s="692" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="703"/>
+      <c r="E53" s="692"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2078470.75</v>
@@ -53775,22 +53808,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="727" t="s">
+      <c r="D54" s="722" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="727"/>
+      <c r="E54" s="722"/>
       <c r="F54" s="111">
         <v>-1448401.2</v>
       </c>
-      <c r="I54" s="704" t="s">
+      <c r="I54" s="693" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="705"/>
-      <c r="K54" s="706">
+      <c r="J54" s="694"/>
+      <c r="K54" s="695">
         <f>F56+F57+F58</f>
         <v>1025960.7</v>
       </c>
-      <c r="L54" s="706"/>
+      <c r="L54" s="695"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -53831,11 +53864,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="708">
+      <c r="K56" s="697">
         <f>-C4</f>
         <v>-754143.23</v>
       </c>
-      <c r="L56" s="709"/>
+      <c r="L56" s="698"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -53852,22 +53885,22 @@
       <c r="C58" s="112">
         <v>44591</v>
       </c>
-      <c r="D58" s="686" t="s">
+      <c r="D58" s="675" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="687"/>
+      <c r="E58" s="676"/>
       <c r="F58" s="113">
         <v>1149740.4099999999</v>
       </c>
-      <c r="I58" s="688" t="s">
+      <c r="I58" s="677" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="689"/>
-      <c r="K58" s="690">
+      <c r="J58" s="678"/>
+      <c r="K58" s="679">
         <f>K54+K56</f>
         <v>271817.46999999997</v>
       </c>
-      <c r="L58" s="690"/>
+      <c r="L58" s="679"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -54011,20 +54044,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="K52:L52"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -54040,6 +54059,20 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="K52:L52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -54049,7 +54082,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -56797,7 +56830,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -56833,7 +56866,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="675"/>
+      <c r="B1" s="699"/>
       <c r="C1" s="741" t="s">
         <v>646</v>
       </c>
@@ -56849,7 +56882,7 @@
       <c r="M1" s="742"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="676"/>
+      <c r="B2" s="700"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -56859,21 +56892,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="679" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="680"/>
+      <c r="B3" s="703" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="704"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="681" t="s">
+      <c r="H3" s="705" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="681"/>
+      <c r="I3" s="705"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="718" t="s">
+      <c r="P3" s="729" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="739" t="s">
@@ -56891,14 +56924,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="682" t="s">
+      <c r="E4" s="706" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="683"/>
-      <c r="H4" s="684" t="s">
+      <c r="F4" s="707"/>
+      <c r="H4" s="708" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="685"/>
+      <c r="I4" s="709"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -56908,15 +56941,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="719"/>
+      <c r="P4" s="730"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="740"/>
-      <c r="W4" s="728" t="s">
+      <c r="W4" s="712" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="728"/>
+      <c r="X4" s="712"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -56967,8 +57000,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="728"/>
-      <c r="X5" s="728"/>
+      <c r="W5" s="712"/>
+      <c r="X5" s="712"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -57729,7 +57762,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="732">
+      <c r="W19" s="716">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -57781,7 +57814,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="733"/>
+      <c r="W20" s="717"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -57830,8 +57863,8 @@
         <v>18072</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="734"/>
-      <c r="X21" s="734"/>
+      <c r="W21" s="718"/>
+      <c r="X21" s="718"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -57930,8 +57963,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="735"/>
-      <c r="X23" s="735"/>
+      <c r="W23" s="719"/>
+      <c r="X23" s="719"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -57986,8 +58019,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="735"/>
-      <c r="X24" s="735"/>
+      <c r="W24" s="719"/>
+      <c r="X24" s="719"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -58035,8 +58068,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="736"/>
-      <c r="X25" s="736"/>
+      <c r="W25" s="720"/>
+      <c r="X25" s="720"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -58084,8 +58117,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="736"/>
-      <c r="X26" s="736"/>
+      <c r="W26" s="720"/>
+      <c r="X26" s="720"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -58133,9 +58166,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="729"/>
-      <c r="X27" s="730"/>
-      <c r="Y27" s="731"/>
+      <c r="W27" s="713"/>
+      <c r="X27" s="714"/>
+      <c r="Y27" s="715"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -58183,9 +58216,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="730"/>
-      <c r="X28" s="730"/>
-      <c r="Y28" s="731"/>
+      <c r="W28" s="714"/>
+      <c r="X28" s="714"/>
+      <c r="Y28" s="715"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -58526,11 +58559,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="720">
+      <c r="M36" s="731">
         <f>SUM(M5:M35)</f>
         <v>2143864.4900000002</v>
       </c>
-      <c r="N36" s="722">
+      <c r="N36" s="733">
         <f>SUM(N5:N35)</f>
         <v>791108</v>
       </c>
@@ -58563,8 +58596,8 @@
       <c r="L37" s="61">
         <v>16518.78</v>
       </c>
-      <c r="M37" s="721"/>
-      <c r="N37" s="723"/>
+      <c r="M37" s="732"/>
+      <c r="N37" s="734"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
@@ -58871,26 +58904,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="697" t="s">
+      <c r="H52" s="686" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="698"/>
+      <c r="I52" s="687"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="699">
+      <c r="K52" s="688">
         <f>I50+L50</f>
         <v>197471.8</v>
       </c>
-      <c r="L52" s="726"/>
+      <c r="L52" s="721"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="703" t="s">
+      <c r="D53" s="692" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="703"/>
+      <c r="E53" s="692"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2057786.11</v>
@@ -58899,22 +58932,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="727" t="s">
+      <c r="D54" s="722" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="727"/>
+      <c r="E54" s="722"/>
       <c r="F54" s="111">
         <v>-1702928.14</v>
       </c>
-      <c r="I54" s="704" t="s">
+      <c r="I54" s="693" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="705"/>
-      <c r="K54" s="706">
+      <c r="J54" s="694"/>
+      <c r="K54" s="695">
         <f>F56+F57+F58</f>
         <v>1147965.3400000003</v>
       </c>
-      <c r="L54" s="706"/>
+      <c r="L54" s="695"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -58955,11 +58988,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="708">
+      <c r="K56" s="697">
         <f>-C4</f>
         <v>-1149740.4099999999</v>
       </c>
-      <c r="L56" s="709"/>
+      <c r="L56" s="698"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -58976,22 +59009,22 @@
       <c r="C58" s="112">
         <v>44619</v>
       </c>
-      <c r="D58" s="686" t="s">
+      <c r="D58" s="675" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="687"/>
+      <c r="E58" s="676"/>
       <c r="F58" s="113">
         <v>1266568.45</v>
       </c>
-      <c r="I58" s="688" t="s">
+      <c r="I58" s="677" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="689"/>
-      <c r="K58" s="690">
+      <c r="J58" s="678"/>
+      <c r="K58" s="679">
         <f>K54+K56</f>
         <v>-1775.0699999995995</v>
       </c>
-      <c r="L58" s="690"/>
+      <c r="L58" s="679"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -59135,6 +59168,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -59151,20 +59198,6 @@
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
     <mergeCell ref="M39:N39"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
   </mergeCells>
   <pageMargins left="0.23" right="0.23" top="0.4" bottom="0.28000000000000003" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>